<commit_message>
upload new dataset file
</commit_message>
<xml_diff>
--- a/mypertaminadata.xlsx
+++ b/mypertaminadata.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Rumah Laptop\Desktop\TA\TA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{31A7AF4D-D97F-472D-94C0-6D1F38B291C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FB56CF23-1BAD-43B6-9242-D5B8D91EEA4A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{4E7733B9-F792-401C-B5DC-AA1060593172}"/>
+    <workbookView xWindow="0" yWindow="600" windowWidth="20490" windowHeight="10920" xr2:uid="{4E7733B9-F792-401C-B5DC-AA1060593172}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -33,20 +33,825 @@
     <t>Saya kasih bintang 5, tpi tolong kasih saya solusi. Saya ada permasalahan gini. Tempo hari ada kalo nggk salah 2 bulanan, di daftarkan my pertamina oleh salah satu karyawan SPBU, terus di suruh nunggu beberapa hari. Selang 1 bulan saya kembali ( ke SPBU tersebut), dan coba log in dengan NIK dan pasword yg sudah didaftarkan. Dan permasalahan nya ketika saya log in subsidi tepat, ada permintaan kode verivikasi dari email yg terdaftar, waktu di cek dari email yg terdaftar tidak ada kode veri masuk</t>
   </si>
   <si>
-    <t>Pelayanan memuaskan waktu bantu bikin.aplikasi subsidi</t>
-  </si>
-  <si>
-    <t>Sudah 1 bulan belum dpt barkot hadeh....</t>
-  </si>
-  <si>
     <t>Jelek dan lelet.... Serta respon layanan sangat lambat</t>
   </si>
   <si>
-    <t>Susah ngisinya ,,,data yang sudah diisi slalu hilang,sudah mau siap di isi data nya,, slalu saja balik ke menu awal...</t>
-  </si>
-  <si>
-    <r>
-      <t>abu mansur1</t>
+    <t>Log-in password lelet minta ampun, aplikasi error kok dipasang, sinyal full bisa mendadak lemot</t>
+  </si>
+  <si>
+    <t>Ribet untuk pengguna yang tidak memakai handphone android</t>
+  </si>
+  <si>
+    <t>PT pertamina memutus rejeki orang eceran minyak, mikir mikir dulu lah sebelum buat aplikasi,</t>
+  </si>
+  <si>
+    <t>Sudah daftar dan berhasil registrasi. Tapi tidak bisa masuk, jaringan bagus tetap tidak bisa masuk. OS android 10 masih tidak bisa masuk. Jadi gimana ini solusinya</t>
+  </si>
+  <si>
+    <t>Aplikasi yang mempersulit hidup rakyat jelata</t>
+  </si>
+  <si>
+    <t>Baik dilaksanakan dgn caraini, tetapi sulit untuk mencapai tujuan kesuksesan bagi rakyat biasa,</t>
+  </si>
+  <si>
+    <t>Beberapa menu aplikasi sering error, tidak ada fitur auto save, semoga hari mu suram</t>
+  </si>
+  <si>
+    <t>Hancur parah. Ringsek. Nyungsep..Ngabisin kuota aja</t>
+  </si>
+  <si>
+    <t>Tidak membantu,malah menmbah susah</t>
+  </si>
+  <si>
+    <t>Enak ya jadi penguasa bikin aturan semaunya,rakyat sudah pusing di tambah pusing lagi..ingat gajimu dari rakyat,,dzolim</t>
+  </si>
+  <si>
+    <t>Gimana nih keterangan maxsimal 2 mb tapi yg di upload 1,5mb trus ada peringatan melebihi kapasitas, sumpah aneh,</t>
+  </si>
+  <si>
+    <t>Aplikasi mengada-ada, nyusahin masyarakat kelas bawah, subsidi itu untuk RAKYAT KELAS BAWAH dimana mereka kebanyakan TIDAK PUNYA ANDROID</t>
+  </si>
+  <si>
+    <t>a sampe 20 kali mendaftar tapi tidak juga bisa terdaftar, entah apa yg salah yg daftarkan petugas pertamina tapi dia gak tau dimana salahnya, sunggu aneh</t>
+  </si>
+  <si>
+    <t>Mau daftar program subsidi tepat trus isi biodata pribadi mau kehalaman selanjutnya tidak bisa sudah daftar ke aplikasinya maupun websitenya tetap tidak bisa ke halaman selanjutnya</t>
+  </si>
+  <si>
+    <t>Di unduh sudah.. Registrasi angele pol²an Klo lom bisa di pake ni aplikasi jgn suruh dulu org² download Ngeselin.</t>
+  </si>
+  <si>
+    <t>Hapus aja aplikasi ini gak bisa di pakai terus di spbu rawa buntu 3515309 buat menejemen spbu rawa buntu jangan alesan terus . Klw pake my pertamina</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Lumayan bagus , di percepat aja proses penggunaan apk nya jangan lemot karena kita lagi di spbu </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>😁</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Harus di daftarkan oleh petugas spbu, daftar sendiri katanya gak bisa atau sangat sulit... Begitu kata petugas spbu. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>😴</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Susah banget daftar nya gila,jaringan gua bagus² gini malah lemot di apk nya heran</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>😑</t>
+    </r>
+  </si>
+  <si>
+    <t>Sebenarnya sangat di butuhkan tapi ribet kalau mau daftar sudah berkali2 coba di websitenya tetap aja gak bisa memang parah pelayannya, padahal di wajibkan pakai, tapi giliran mau daftar bikin susah payah</t>
+  </si>
+  <si>
+    <t>Mantap aplikasi nya tpi seharusnya Ada komentar tentang SPBU pengisian nya nilai dan buruk SPBU di lapangan</t>
+  </si>
+  <si>
+    <t>Parah untuk pendaftaran BBM subsidi, sistem selalu gagal, ketika menghubungi call center selalu sibuk, padahal telpenggunakan pulsa pribadi, .</t>
+  </si>
+  <si>
+    <t>plikasi jelek sangat membingungkan</t>
+  </si>
+  <si>
+    <t>Aplikasi gajelss, buat mempersulit masyarakat, barang siapa yang mempersuliat urusan orang lain, maka hidup nya akan di persulit oleh allah swt</t>
+  </si>
+  <si>
+    <t>Jelek berusaha daftar tapi link hilang 2 terus.bikin darah tinggi</t>
+  </si>
+  <si>
+    <t>Saat masuk pada hkaman qr barcode selalu possward tidak sesuai padahal sudah sesuai sama pendaftaran awal</t>
+  </si>
+  <si>
+    <t>Bikin ribet doang ujung ujungnya BBM naik</t>
+  </si>
+  <si>
+    <t>Meresahkan rakyat yang sudah lansia</t>
+  </si>
+  <si>
+    <t>Kita lihat aja dulu, apa alasan pertamina harus pakai aplikasi utk isi BBM</t>
+  </si>
+  <si>
+    <t>Alhamdulillah dgn aplikasi mypertamina,dpt mendptkan bbm bersubsidi dgn tepat</t>
+  </si>
+  <si>
+    <t>Petinggi yang berbuat rakyat yang bertanggung jawab.. ekonomi rakyat kecil yg awam gak bisa berkembang dgn di persulitnya BBM.</t>
+  </si>
+  <si>
+    <t>Bad banget, buat ngisi daftar subsidi balik balik sendiri</t>
+  </si>
+  <si>
+    <t>ngk jelas, udah daftar d website nya, eh malah mau login pw nya salah mulu. . giliran mau d ganti malah email nya ngk masuk"</t>
+  </si>
+  <si>
+    <t>Maksud memudahkan rakyat, semoga maksud itu tercapai..</t>
+  </si>
+  <si>
+    <t>gimana ya bos caranya habis masukin nik trus pasword munculnya gitu gitu aja</t>
+  </si>
+  <si>
+    <t>Selalu dipaksakan..... Dari awal sampe sekarang utk daftar kendaraan g bisa app rongsok</t>
+  </si>
+  <si>
+    <t>Sungguh menyusakan dan tidak efektif.apa lagi buat kita yang di daerah papua . aplikasi nya sangan tidak optimal...dan tidak bisa si daftar</t>
+  </si>
+  <si>
+    <t>Bodoh banget ayowadah pembayaran diperluas lgi,tdk semu customer memiliki hp android dg kapasitas yg baik. Blm lagi harus memerbarui versinya stiap masanya. Inovasi d era berkembangan digitalnya dpt, tp Lebih merakyaaat laaaah. Di indonesia masih banyak wong cilik.</t>
+  </si>
+  <si>
+    <t>Saya udah login tapi beberapa hari kemhdian kok login an saya g bisa lagi ya</t>
+  </si>
+  <si>
+    <t>Saya kasih 2 bintang saja Masa sampai sekrang mendatar pengguna Bio solar bersubsidi erorr trus ribet banget bisa gx bikin aplikasi bodh</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mempersulit dan meribetkan yg sudah mudah </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤭</t>
+    </r>
+  </si>
+  <si>
+    <t>Untuk mendaftar program subsidi tepat...susah, selalu logout sendiri sangat bikin susah rakyat!!!!!!!</t>
+  </si>
+  <si>
+    <t>Duh udah daftar cari yg bisa spbu gak suport smua. My pertamina. Sayang udah ngisi saldo kaga kepake. Aturan mah suportin dulu semua spbu baru bikin aplikasi.</t>
+  </si>
+  <si>
+    <t>Kenapa subsidi jikalau dipaksa harus membeli nonsubsidi? Antrian sekarang semakin panjang, alasan bangkrut padahal gak ada saingan.tidak berlaku bodoh</t>
+  </si>
+  <si>
+    <t>Di permudah karena masih banyak yang belum tahu</t>
+  </si>
+  <si>
+    <r>
+      <t>Aplikasi yang sangat berguna bagi masyarakat banyak kususnya para petani Dan nelayan buat pembelian bahan bakar solar dan pertalit buat mesin desel sawah dan buat bahan bakar mesin perahu</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>😊🥰</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Sungguh bagus dan bermanfaat...makasih my Pertamina </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍👍</t>
+    </r>
+  </si>
+  <si>
+    <t>Apk busuk skali buat daftar aja susah. Terus bagaimana seharusnya...bikin ribet orang aja...beli BBM aja pake aplikasi...bikin ribet bikin macet nantinya hadeh...ada2 aja ini aturan</t>
+  </si>
+  <si>
+    <t>Pendaftaran di aplikasi ini ditolak ikarena nama kelurahan TIDAK TERISI, dikarenakan pada option KELURAHAN TIDAK TERDAFTAR. Adapun nama kelurahan yang dimaksud/tidak ada optionnya adalah Kelurahan PESU Kec. Wedi, Kab. Klaten, Prov.Jateng</t>
+  </si>
+  <si>
+    <t>Menggunakan aplikasi MyPertamina sangat lah praktis dan tdk ribet.</t>
+  </si>
+  <si>
+    <t>Wow sangat bermaanfaat sekali bagi masyarakat lebih efisian sekali……</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Biasanya aplikasi untuk memudahkan, ini malah nyusahin </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🤬</t>
+    </r>
+  </si>
+  <si>
+    <t>Di spbu ga bisa pakai hp. Ehhh bikin riwehh baeeeeee</t>
+  </si>
+  <si>
+    <t>Hari ini sebagian dikota Banjarbaru diberlakukan mypertamina sangat lah mudah pengisiannya di SPBU .tidak dikuasi oleh pelangsiran lagi singga anggutan umum bisa ngisi dengan mudah pake aplikasi mypertamina.kami ucapan kan terimakasih kepada pemerintah sudah memberlakukan mudah mudahan minyak subsidi tepat sasaran sebagai mana harapan pemerintah</t>
+  </si>
+  <si>
+    <t>Kasih 1 dulu,biar semangat update videonya biar makin kocak,kalau menurutsaya tambahin dong efek recallnya sama edit video gamenya..</t>
+  </si>
+  <si>
+    <t>Semoga menjadi aplikasi terbaik</t>
+  </si>
+  <si>
+    <t>Kalo beli bmm di bus simulator harus pakai Mypertamina dulu</t>
+  </si>
+  <si>
+    <t>Ini gak bisa konekin Link Aja. Udah 2 bulan masa gak beres2 masalahnya</t>
+  </si>
+  <si>
+    <t>Bisa gak ya pembayarannya jangan paki link aja? Pake kartu debit kek..gak semua org punya dompet digital...dan gak semua orang hp nya punyab kapasitas mumpuni untuk menyimpan berbagai aplikasi..</t>
+  </si>
+  <si>
+    <t>Kira kira ada ga ya penilaian minus lima? Kebijakan bodoh dengan aplikasi bodoh. Beli gas dan BBM aja ribet. Tapi ya maklum otak mereka prinsipnya kalau bisa dipersulit kenapa harus dipermudah?</t>
+  </si>
+  <si>
+    <t>Beli bensin pakai apk. Daftar nya di apk aja susah nya minta ampun.</t>
+  </si>
+  <si>
+    <t>pload data sampai 30 menit gak selesai. Untuk yang mau daftar subsidi tepat, siapin KTP, STNK. Banyak data yang diminta. Perbaiki server datanya. Masak perusahaan Forbes 500 upload data 30 mnt gak selesai.</t>
+  </si>
+  <si>
+    <r>
+      <t>Aplikasi ngk jelas. SDH memasuka data,foto dsb. Sdh nyampe foto2 STNK sama kendaraan. Pas klik kembali lngs balik ke beranda. Padahal belum selesai Ini bagaimana sihhh. Bikin repoot aja.</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👎👎</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> Sdh bolak balik nyoba Kya gitu terus. Payaah</t>
+    </r>
+  </si>
+  <si>
+    <t>Sudah daftar subsidi tepat dari pertama kali, tpi sampai sekarang ga bisa d claim karena password salah, udah reset pass tpi ga ada email yg masuk, daftar lg juga ga bisa! Padahal mobil 1000cc.. Komplain ke cs ga ada tanggapan!! Subsidi tepat mungkin hanya wacana menaikkan harga bbm biar masyarakat g gaduh nantinya!</t>
+  </si>
+  <si>
+    <t>Merepotkan bapak saya, yg mobilnya calya, itupun dibuat angkut kelapa (kulakan). Btw bapak saya cuma jual kelapa di pasar di bangkalan madura. Bapak gaptek. Sedang beli bengsin harus pakai ini kalau kulakan kelapa di surabaya. Bener bener repot aku ngajarinnya</t>
+  </si>
+  <si>
+    <t>Aplikasi ribet ,dikira orang" awam bisa pake aplikasi ini ,udah idup sulit dibikin tabah sulit aja ,kasian mak gw noh mau beli bensin aja suruh mikir keras buat belajar ginian</t>
+  </si>
+  <si>
+    <t>Prnh nukar point dgn jaket+replika SPBU dan replika truk Tanki tapi g di kirim</t>
+  </si>
+  <si>
+    <t>Aplikasi tidak pro rakyat, gimana rakyat kecil yg tidak punya android?</t>
+  </si>
+  <si>
+    <t>Kasi bintang 1 dulu. Aplikasi plat merah buruk dan memaksa</t>
+  </si>
+  <si>
+    <t>Aplikasinya berat bukanya, tdk smua android suport</t>
+  </si>
+  <si>
+    <t>Padahal sudah beli skin tapi tidak masuk". Hmm aplikasinya sih bagus tapi ya gtu sudah beli tapi tidak di tanggapi. Saran juga natalia jgan hilang" gitu dong kan susah untuk nge hitnya. Masa selesai mukul langsung hilang</t>
+  </si>
+  <si>
+    <t>BBM susah daftar data sudah lengkap juga masih susah udah berulang ulang tapi ga bisa daftar juga Sebenarnya mau nya pemerintah itu gimana yah kok makin mempersulit begini</t>
+  </si>
+  <si>
+    <t>tadinya app ini bagus smpe mas² operator nosel bilang "sudah tdk ad lagi jalur my pertamina" harus ikut antrian panjang... kecewa</t>
+  </si>
+  <si>
+    <t>Belum bisa beli pertalite untuk motor disemua spbu pertamina Dan yang biasanya bisa, sekarang malah jadi gak bisa, kata petugasnya hanya untuk mobil yang diprogramkan subsidi saja yang bisa</t>
+  </si>
+  <si>
+    <t>Aplikasi ndk guna bikin bingung masyarakat.klu naik ndk USA membingungkan.pikirin rakyat ya pejabat</t>
+  </si>
+  <si>
+    <t>Untuk aplikasi nya sudah bagus cuman grafik nya agak burik sama sama</t>
+  </si>
+  <si>
+    <t>Untuk pihak program MyPertamina saya minta tolong untuk proses verifikasi setelah pendaftaran dilakukan agar secepatnya diterima,agar kami bisa sesegera mungkn mendapatkan Kode QR (Barcode). Hanya karna blm diverifikasi sampai saat ini saya sudah 3 hari kesulitan mendapatkan BBM.,jadi saya mnta tolong bantu kami dengan cara mempercepat proses pengambilan barcodw untuk pendaftar baru.temksh ..</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Suruh pake aplikasi tapi pembayaran hanya terbatas di satu pembayaran aja, kalo udh wajib harusnya metode pembayaran ya bisa semua tetapi sudah sangat membantu </t>
+  </si>
+  <si>
+    <t>Buruk sekali...tidak bisa dapat melanjutkan perintah setelah tersimpan data pribadi...gimana nih... kejam</t>
+  </si>
+  <si>
+    <t>Aplikasi tolol tanggal lahir gw salah tauan siapa gw apa lo... Beli bensin aja ribet... Naikin terus harga nya</t>
+  </si>
+  <si>
+    <t>INI MAH MEMPERSULIT BUKAN MEMPERMUDAH.BANGSATTTTT!!!!!!!!!</t>
+  </si>
+  <si>
+    <t>Mohon kepada owner aplikasi, ditempat saya sudah di perlakukan aplikasi my Pertamina.. dan saya sudah download dan mau daftar sudah mengisi data diri lengkap saya pencet selanjutnya tidak bisa .. mohon kepada owner aplikasi nya . Ini kenapa ya?</t>
+  </si>
+  <si>
+    <t>INI sangat cocok untuk pembelian BBM</t>
+  </si>
+  <si>
+    <t>Aplikasi N**ntot! Mempersusah untuk isi bensin!</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">mau claim QR code susah nya kaya nyari keadilan di negeri ini. bukannya di bikin mudah, malah di bikin ribet </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🖕🖕🖕🖕</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Mengikuti peraturan yang berada saat ini </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>😎</t>
+    </r>
+  </si>
+  <si>
+    <t>Rumit sangat tidak membantu, metode klaim pembayaran cuma pakai link aja, seharusnya ditambahkan aplikasi lainnya jangan link aja, saya curiga ada permainan apa disini, meribetkan rakyat kecil yg tidak paham dan tidak bisa menggunakan aplikasi, nanti subsidibya cuma untuk org yg berduit saja, ribet untuk semuanya</t>
+  </si>
+  <si>
+    <t>Dafar My Pertamina. Caranya Mendapatkan aplikasi my pertamima</t>
+  </si>
+  <si>
+    <t>Aplikasinya sudah bagus tapi kebijakannya konyol jadi bintang 1.</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">Kasih 2 </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>🌟🌟</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t xml:space="preserve"> dulu soalnya belum tahu manfaat ke depannya bagaimana</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>Dengan aplikasi MyPertamina</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <color theme="1"/>
+        <rFont val="Segoe UI Emoji"/>
+        <family val="2"/>
+      </rPr>
+      <t>👍👍</t>
+    </r>
+  </si>
+  <si>
+    <t>Masih ada banyak kekurangan / ada banyak sekali bug dan mempersulit bagi pengguna aplikasi nya tolol yang bikin</t>
+  </si>
+  <si>
+    <t>Tolong di batasin donk pembelian pertalite yg menggunakan kapasitas besar</t>
+  </si>
+  <si>
+    <t>text</t>
+  </si>
+  <si>
+    <t>,1,2022-07-15 23:29:56,"Semoga aplikasinya cepat diperbaiki, karena begitu banyak masalah saat menggunakan aplikasi ini, setidaknya jangan membuat kami tambah susah,karena kami udah sangat susah."</t>
+  </si>
+  <si>
+    <t>,5,2022-07-16 08:02:23,Bermanfaat banget kalau mau tracking pengeluaran bbm</t>
+  </si>
+  <si>
+    <t>,1,2022-07-16 08:31:23,Ribet lu isi bensin aja ribetðŸ‘Ž</t>
+  </si>
+  <si>
+    <t>,1,2022-07-16 11:41:40,Aplikasi payah...lelet...ðŸ‘ŽðŸ‘ŽðŸ‘ŽðŸ‘Ž</t>
+  </si>
+  <si>
+    <t>01:59:22,aplikasi yang Sangat Merepotkan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01:57:22,Tidak Berguna Dan Sangat Merepotkan</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02:06:11,"Awalnya terasa Ribet, Seiring Waktu Semakin Praktis, Jaya Selalu Pertamina."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02:24:23,Aplikasi yang sangat bagus &amp; sangat mempermudah saat bertransaksi. Terima kasih MyPertamina ðŸ‘ðŸ‘ðŸ‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02:49:05,Kembali ke normal lagi tanpa aplikasi ðŸ¤²</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04:28:31,Setelah diupdate baru bisa buka aplikasi MyPertamina. Waktu mau daftar kendaraan sesuai kemauan pemerintah tidak bisa masukan data2. Saya tambah satu bintang saja.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 05:55:27,Konfirmasi datanya lama Keburu behan bakarnya habisðŸ˜ ðŸ˜ ðŸ˜ ðŸ˜</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 07:09:09,Ø§Ù„Ø­Ù…Ø¯ Ù„Ù„Ù‡ Alhamdulillah Bagus Good</t>
+  </si>
+  <si>
+    <t>iya!!!!!!ðŸ‘‰ðŸ‘ŒðŸ‘‰ðŸ‘ŒðŸ‘‰ðŸ‘ŒðŸ‘‰ðŸ‘ŒðŸ’¦"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14:09:53,"buat pertamina, saya dukung program nya.. maju terus, memang mengubah kebiasaaan itu susah.. tpi nanti lama2 klo udah terbiasa juga bisa diterima"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17:59:51,aplikasi buat susah banyak spam bug dll hadeh payah ne aplikasi.. tolong hapus saja aplikasi ini sangat tidak menolong</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23:37:52,Kebanyakan aturan ribet banget anjg bikin orang tambah susah njg!!!!!</t>
+  </si>
+  <si>
+    <t>18 00:00:11,Sangat membantu sekali karna saya dapat membeli bbm dengan mudah tanpa harus membawa uang cash..,,</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04:00:01,Dukung kemajuan Indonesias</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 05:01:03aplikasi my,Pertamina mantap</t>
+  </si>
+  <si>
+    <t>10:52:00Aplikasi sampah, udah terferifikasi dari bulan juli qr code dah dapet, ganti hp malah gabisa claim qr code lagi, APLIKASI SAMPAH !!!ðŸ—¿</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 09:12:13,Nyobain tadi bayar bensin pake app ini. Udah di isi 21 rebu. Eh pas mau bayar aplikasi nya coba lagi coba lagi Mulu. Ampe setengah jam ngotak ngatik ini aplikasi. Padahal jaringan bagus. Mana kaga bawa duit. Parah dah. Malu maluin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10:40:30,Mempersulit rakyat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10:54:20,Udah daftar buat kode qr udah seminggu lebih tapi gak diverifikasi</t>
+  </si>
+  <si>
+    <t>18 07:13:35,Tidak bisa login padahal udah daftat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11:06:11,Aplikasi yg tidak perlu sangat sangat bodoh yg menyatankan aplikasi ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11:44:11,"Sistem apaan ini?? Yg ngasih bintang lima gak ada otak, anjg!"</t>
+  </si>
+  <si>
+    <t>1,2022-07-18 11:50:15,Mohon perbaikannya terlalu banyak bug apalagi saat bertemu tiba tiba sat set swing.... Grafis Nya mohon di tingkat kan lagi sayang banget game sebagus ini banyak bug nya....</t>
+  </si>
+  <si>
+    <t>1,2022-07-18 12:08:16,Entah ini apk buat apa gajelas</t>
+  </si>
+  <si>
+    <t>1,2022-07-18 12:26:18,Semoga bbm harganya turun amin</t>
+  </si>
+  <si>
+    <t>02:00Bikin ribet, mau menghubungkan ke link saja tidak bisa dengan alasan waktu habis, bikin aplikasi apa ini sangat jelek sekaliðŸ˜‘ðŸ˜‘ðŸ˜‘ðŸ˜‘</t>
+  </si>
+  <si>
+    <t>02:50:41,Bagus sekali aplikasinya sangat membantu dan lebih efektif serta efsien,……</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:02:42,Keren dan mempermudah,  inovatif salam sukses</t>
+  </si>
+  <si>
+    <t>03:07:56,Sangat memuaskan... Kedepan lebih mudah dan bermanfaat.. ðŸ‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:38:22,Mantapdan lebih efisen </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 06:16:22,"Sebenarnya tujuannnya bagus, tapi langkahnya mungkin kurang efektif, ya. My pertamina sudah bisa mengambil data ribuan kendaraan dari aplikasi transportasi, katakan kerjasama pemberian barcode. Sisanya tingal yg tidak ada aplikasi transportasi. Selain itu, masyarakat agak curiga ini aplikasi akal2an guna menaikkan aplikasi Link aja. Karena kalo mau adil semua metode pembayaran ovo, gopay dan yg lain harus bisa di integrasikan. Terima kasih semoga masukan kami bermanfaat."</t>
+  </si>
+  <si>
+    <t>09:28:35,Tolong permudah pembayaran via gopay atau ovo....terima kasih.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12:05:12,Untuk aplikasinya udh cukup bagus ya intinya di permudah aja dalam pembayaran Pokoknya bagus lah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:02:42,Keren inovatif salam sukses</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:07:56,Sangat memuaskan... Kedepan lebih mudah dan bermanfaat.. ðŸ‘</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:27:46,Pakai mypertamina sangat praktis.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 07:34:48,"Setelah sekian lama daftar baru dapat notifikasi dan QR codenya. Scara penggunaan aplikasi myPertamina dapat mudah dilakukan di kota besar. Sekarang tinggal masalah di ketersediaan pertalite-nyaðŸ˜“. Beberapa kali masuk SPBU, pertalite kosong"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11:28:20,Kalau untuk tujuan tepat sasaran pemakai bbm subsidi sih ok. Cuma cara menggunakan agar bisa lebih di permudah</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12:17:28,Mohon pihak playstore dan Stade holder terkait karena menyusahkan masyarakat kalangan bawah dan menengah dan mengajukan keberatan dengan aplikasi my Pertamina karena sistem login menggunakan nomor ponsel pengguna akun lainnya dan serta pin rekening bank ini bisa mempermudah hacker mencuri data pengguna akun lainnya di seluruh Indonesia dan menggunakan password yang belum aman dari sistem keamanan yang menjamin pengguna akun lainnya di seluruh Indonesia dan mohon diblokir aplikasi my Pertamina</t>
+  </si>
+  <si>
+    <t>21:17:00aplikasi yang sangat buruk untuk pelayanan masyarakat ,hanya untuk merubah data kendaraan saja sudah 2 hari tidak bisa diupdate!!</t>
+  </si>
+  <si>
+    <t>00:18:00Aplikasi tidak ada guna nya kebanyakan tidak bisa di gunakan seluruh pertamina..kapan di tanya pagi tidak bisa,kapan di tanya malam tidak bisa..terus kapan bisa...tolong tegas buat kebijakan nya..jangan buat kebijakan tidak tegas dan tidak bermutu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04:43:25,semoga sesuai dengan tujuan bagi yang berhak mendapat subsidi bbm</t>
+  </si>
+  <si>
+    <t>04:44:18,Semoga subsidi BBM tepat sasaran</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 05:50:45,Gak guna... Unsinstall aja lah</t>
+  </si>
+  <si>
+    <t>06:02:00Jadi begini masalahnya, ketika Saya tidak membawa uang cash, maka saya sangat tergantung dengan aplikasi my pertamina. Tapi yang sangat mengecewakan adalah ketika sudah selesai isi pertamax, ternyata pembayaran menggunakan mypertamina malah gangguan. Nah ini sangat memalukan sekali….apalagi saat tidak membawa uang cash. Saya sudah berkalikali di permalukan sama aplikasi ini karena setiap akan melakukan pembayaran, selalu mengalami gangguan dan akhirnya harus ambil uang diu atm. ðŸ˜ðŸ˜µðŸ˜¡</t>
+  </si>
+  <si>
+    <t>08:51:49,"Gk boleh make hp di SPBU, tapi disuruh download aplikasi terus make si SPBU,"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 09:34:58,APLIKASI TIDAK BERGUNA!!!!</t>
+  </si>
+  <si>
+    <t>09:35:19,Merepotkan warga desa seperti saya</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 09:38:05,Aplikasi tidak bagus. Berbelit. Aplikasi pura pura hanya untuk menutupi program yang lain</t>
+  </si>
+  <si>
+    <t>10:00:22,Aplikasi tidak layak pakai</t>
+  </si>
+  <si>
+    <t>12:40:00Untuk aplikasi sih sudah mantap...hanya saja sayangnya tidak di gunakan dengan baik oleh para SPBU,bisa di katakan untuk sekarang SPBU masih lebih suka dengan uang</t>
+  </si>
+  <si>
+    <t>10:08:01,Tidak sebagus my pertamina unlimited mode</t>
+  </si>
+  <si>
+    <t>10:14:32,"Tidak bisa tersambung, susah di pake di spbu gak boleh mainan hp"</t>
+  </si>
+  <si>
+    <t>10:22:06,"Ini sebenarnya pertamina niat gak sih bikin aplikasi, sudah berhari-hari error terus. dikasih waktu tenggang sampe 30 Juli. Perusahaan bumn besar urusan aplikasi aja sampe kaya gini banget."</t>
+  </si>
+  <si>
+    <t>10:37:33,"Saat mengisi data tanggal lahir, anehnya bulan Februari tidak bisa dipilih. Saat memilih Februari, yang muncul di pengisian malah Januari. Mohon dikoreksi, terima kasih."</t>
+  </si>
+  <si>
+    <t>11:22:36,"Subsidi biar tepat sasaran.... Mantabs, maju terus pertamina. NKRI harga mati.."</t>
+  </si>
+  <si>
+    <t>11:34:01,Mempersulit rakyat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12:05:01,"Gini orang suruh pake, udah ribet, error gobblk pula, link aja juga sama gblknya bikin malu aja pas scan gagal terus aplikasi sialan"</t>
+  </si>
+  <si>
+    <t>12:22:53,"Aplikasi kurang siap masa tiap masuk aplikasi harus masukin password dulu, padahal password udah disimpan aplikasi."</t>
+  </si>
+  <si>
+    <r>
+      <t>03:48:00</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="12"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+      </rPr>
+      <t>Daftarnya ribet, iklan diawal sangat mengganggu, ui/ux tidak responsif</t>
+    </r>
+  </si>
+  <si>
+    <t>01:03:22,Aplikasi buruk sekali</t>
+  </si>
+  <si>
+    <t>01:01:56,Udah susah jadi tambah susah</t>
+  </si>
+  <si>
+    <t>00:58:25,Semenjak saya install MyPertamina . wah hidup saya makin bervariasi ini aplikasi benar benar membayar tanpa iklan . mainkan terus aplikasinya agar hidup anda menjadi beban . ingat saat hidup tidak ada beban andalah yg menjadi beban . secara virtual aplikasi ini sangat virtual . semangat MyPertamina . gtafis sangat lancar . mantabbbb .</t>
+  </si>
+  <si>
+    <t>08:26:00Kok payah x dapat email nya otp nya . . . Bantu lah . Lalap sedikit 2 nik salah n pasword salah apa nya ni app ?</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00:05:01,Mempersulit hidup orang yang udah sulit. Harus dihubungkan dengan link aja. Udah tahu gak semua HP memdai.</t>
+  </si>
+  <si>
+    <t>23:31:43,Aplikasi apa ini nik tidak terbaca</t>
+  </si>
+  <si>
+    <t>23:41:43,Entah lah susah di jelaskan....ribeet…</t>
+  </si>
+  <si>
+    <t>23:45:23,Selevel negara kok tidak mampu bikin aplikasi yang baik. Udah daftar ulang2 tapi tidak bisa login karena no HP/PIN salah. Padahal sudah masukkan dgn benar. Bisa tidak sih negara tidak persulit rakyat sendiri?</t>
+  </si>
+  <si>
+    <t>tidak semua konsumen punya smartphone....beli bbm kok ribet....infrastruktur jaringan internet juga belum merata..... Negara seharusnya mengayomi dan menjamin hidup rakyatnya, bukanya malah berbisnis dengan rakyat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 00:00:53,"Maaf kasih 1 bintang karena engga epektif, malah tambah ribet. Mau daftar susah masuk."</t>
+  </si>
+  <si>
+    <t>12:34:03,"Aplikasi yang menyusahkan manusia Kata nya di pom bensi gk boleh main hp Ini kok di izin ini bukak hp? Gimana kalau pom itu kebakar oleh kita bukak hp emang ad garansi kah misal nya kami kenapa"" oleh ledakan minyak?"</t>
+  </si>
+  <si>
+    <t>11:46:00Susah penggunaannya. Beberapa kali mau beli bensin lewat aplikasi biar bisa dapat poin loyality susah, ditanya ke pegawainya bilangnya ini itu lah. Ga ada petunjuk yang jelas</t>
+  </si>
+  <si>
+    <t>06:37:00Aplikasi yang buruk sekali... Foto bolak balik stnk tetap tidak terbaca.. Padahal jelas sekali fotonya.. Sehingga menghambat pendaftaran…</t>
+  </si>
+  <si>
+    <t>10:53:42,Contoh aplikasi yang menyengsarakn rakyat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02:51:00enak si pakai aplikasi, tidak ribetÂ² bawa uang Cash, semua serba digital, tapi gk ada casehback 25%, padahal di Sticker SPBU terpampang casehback nya ðŸ˜</t>
+  </si>
+  <si>
+    <t>10:06:38,Sangat menyenangkan tidak usah mengeluarkan uang tinggal keluarkan hp dan di tunjukkan aplikasi my pertamina sudah selesai asal saldonya cukup</t>
+  </si>
+  <si>
+    <t>09:32:01,Ini apaan sih daftarin kendaraan capek2 di email sudah di aprov tapi login gagal mulu yg nik gak sama yg nopol gak kedaftar... Daftar lagi udah engga bisa nik terdaftar... Bukan nya bikin simple malah bikin males yang ada</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 09:03:46,"Buat kebijakan harus di pikiri sebelum di laksanakan , jangan ambil keputusan meliat dari posisi kamu berada , liat dari sekitar dan secara luas juga."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 07:02:20,"Aplikasi kayak gini mau di wajib? Sering error pas pembayaran, tidak praktis sama sekali! Perbaiki lah pembayaran harus melalui linkajah, tapi suka error."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 06:40:46,Saya sebagai sopir angkot dan saya gaptek tehnologi dan saya secara tidak langsung di paksa harus beli hp androit sebagaimana fungsinya untuk membeli bensin dan saya terpaksa harus hutang demi membeli hp utk kebutuhan hidup karena anak saya 3 dan sekolah semua</t>
+  </si>
+  <si>
+    <t>02:25:00 Bagus cara mendaftar gampang bagi yang sudah tau. cuma untuk pendaftaran diaplikasi kadang bermasalah. Alternatif lain bisa diweb SUBSIDI TEPAT. Terkadang ada Hp yang tidak support dengan aplikasinya. Untuk Edit data Lebih bagus di aplikasi karena diweb sering bug. Web hanya (untuk daftar) 1. centang 2.pilih daftar sekarang. 3.isi data pendaftaran 4.disini ukuran foto tidak boleh dari 2 MB (harus di kompres). 5.untuk kode verifikasi akan dikirim melalui email.</t>
+  </si>
+  <si>
+    <t>15:32:00Aplikasi macam apa, saya sudah daftar kemaren masak sekali update aplikasinya saya harus daftar balik. Kan tai itu. Masak barcode saya hilang di apliaksinya harus daftar kembali. Aplikasi macam apa ini</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:40:23,Aplikasi apaan sih. Login tidak bisa daftar tidak bisa. Cacat.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02:54:33,"Aplikasi tidak jelas,masa sinkronin ke metode pembayarannya aja tidak bisa bisa..."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02:33:33,"Aplikasi pembodohan, yakali disave tidak bisa tulisan tidak ada jaringan, tekan kembali juga kembali ke awal ngulang lagi dari awal sampe ngulang 5x tetep aja tidak bisa ckckck"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 01:41:42,"Pelayanan menggunakan MyPertamina selama saya pakai ini untuk pengisian bensin motor di SPBU Pertamina sangatlah bagus, praktis juga pelayanan petugas SPBUnya sangat ramah sekali. Dan banyak hadiah yang bagus bagus untuk setiap pembelian bensin. Sudah dapet bensin ++++ dapet kupon poinnya yang bisa ditukarkan berupa hadiah yang bagus sesuai dengan poin kita. Mohon untuk ditingkatkan terus pelayanan MyPertamina untuk kedepannnya lebih bagus &amp; hadiahnya yang keren keren.... Terima kasih ðŸ™"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22:47:41,Daftar program subsidi tidak bisa terus...payah nih aplikasi</t>
+  </si>
+  <si>
+    <t>21:42:00,BIKIN RIBET AJA PAKAI APLIKASI. LEBIH ENAK BAYAR TUNAI!!! NO DEBAT!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16:27:13,Mantap sekali aplikasinya ðŸ‘</t>
+  </si>
+  <si>
+    <t>02:29:00Aplikasi tidak berguna!!! Daftar susah, nelpon call center ketus, belum selesai ngomong udah di sela!! Aplikasi tidak ada berguna!!!</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14:50:18,"Tidak efektif, udah jelas ada tanda hp dilarang malah main hp jadinya di spbu, tidak jelas juga kegunaannya untuk apa ðŸ‘Ž"</t>
+  </si>
+  <si>
+    <t>12:05:12,Untuk aplikasinya udah cukup bagus ya intinya di permudah aja dalam pembayaran Pokoknya bagus lah</t>
+  </si>
+  <si>
+    <t>15:02:25,Aplikasi tidak berguna babi anjing tai bangsat celeh asu sia anjing aplikasi menyulitkan masyarakat bangsat anjing sia anjing yang buat pekok tolol goblok lulusan tk</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 04:43:53,"Niat mempermudah, tapi hasilnya mempersusah masyarakat, aplikasinya tidak berbobot, di perbaikannya, dan sebagai masukan Kalau E-walet ya jangan cuma satu saja donk, dan juga apakah pihak pengembangan sudah memikirkan bagai mana bagi orang-orang tua yg kurang paham pakai android, atau yang engga punya HP android... Kan jadi susah, kasiahan mereka yang tidak punya android dan tidak paham android."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 03:40:25,Terimakasih sudah terdaftar sebagai penerima bbm bersubsidi. Bintang 3 dulu ya</t>
+  </si>
+  <si>
+    <t>13:00 App tersebut sudah sangat mendukung transaksi non tunai, tp ada bbrp SPBU masih bayar dlu baru isi BBM, bukannya kebalikan berapa ril di Isi baru bayar, ðŸ™</t>
+  </si>
+  <si>
+    <t>10:00aplikasi yang sangat tidak berguna, membingungkan mutar-muter bertele-tele.</t>
+  </si>
+  <si>
+    <t>03:40:25,Terimakasih sudah terdaftar sebagai penerima bbm bersubsidi sangat. Lah baik</t>
+  </si>
+  <si>
+    <t>1,2022-07-18 12:12:41,Merepotkan sekali, sangat bodoh aplikasi nya anjing lah…..</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 08:57:00,Sudah terkonfirmasi saat claim qr code muncul belum terverifikasi bagaimana neh payah.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 07:14:56,sudah mengisi identitas. Nggk bisa daftar2. Susah. Di suruh upload foto tp nggk bisa buat upload. Cma hitam tok di layar.. Aplikasi belum benar siap tapi sudah di paksakan.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 02:40:34,"Susah dioperasikan, sering ngelag, error terus, tidak memuaskan pokoknya,"</t>
+  </si>
+  <si>
+    <t>04:04:13,Hmmm tadi coba isi bensi dan bayar pakai mypertamina erorr saat mau pembayaran alhasil pakai cash...</t>
+  </si>
+  <si>
+    <t>12:26:27,"My pertamina sendiri belum siap kok. Malas sekali"asak sudah ngulang 10 kali kok tetap ""ada gangguan dan tidak bisa diinput engga jelas sekali"</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10:46:06,My pertamina bikin ribet menurut saya Kenapa harus pakai pertamina Bagus seperti dulu saja Harus nya indonesia Bukan masalah BBm nya yang di persulit Tapi kendaraan nya jangan setiap tahun Diproduksi tambah macet jadi nya Enak jaman dulu ga banyak kendaraan Sekarang 80% jadi rawan kecelakaan Karena kebanyakan pemotor/yang bermobil Yang masih ambigu atau yang sudah tua juga naik motor/mobil sendiri bagaimana engga habis minyak bumi Kalau kendaraan setiap tahun ditambah terus</t>
+  </si>
+  <si>
+    <t>23:29:56,"Semoga aplikasinya cepat diperbaiki, karena begitu banyak masalah saat menggunakan aplikasi ini aplikasi ini, setidaknya jangan membuat kami tambah susah, karena kami udah sangat susah."</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 09:34:56,"SEMANGAAAT MY PERTAMINAAA, terus berkembaang yaðŸ¥³. Bisa yok bisa. sUdh banyak yang make sistem aplikasi di beberapa tempat tertentu contoh nya bpjs kesehatan(jkn mobil) Bpjs ketenagakerjaan(jmo mobile) dan saya pribadi merasa sangat terbantu dengan kemudahan yang di berikan jadi segala nya bisa lewat hp saja"</t>
+  </si>
+  <si>
+    <t>:06:00Daftar dan menghubungkan ke link aja cepat ga nyampe 5 menit ðŸ‘ðŸ»ðŸ‘ðŸ» semoga untuk kedepan tidak ada kendala</t>
+  </si>
+  <si>
+    <t>,1,2022-07-16 14:14:19,Pertamina tolol udah tau yang isi bensin motor kebanyakan orang tua kamu pikir semua orang tua tau apa cara memakai ini aplikasi</t>
+  </si>
+  <si>
+    <t>,1,2022-07-16 12:14:53,"selalu ditunggangi dengn kepentingan"" yang menguntungkan beberapa pihak ðŸ˜” aku menyebutnya MIRIS &amp; KONYOL"</t>
+  </si>
+  <si>
+    <t>,5,2022-07-16 04:16:15,"Aplikasi MyPertamina wajib dimiliki untuk kemudahan transaksi pembelian BBM diseluruh Indonesia, sangat mudah mengoperasikan dan terintegrasi dengan data kita"</t>
+  </si>
+  <si>
+    <t>,1,2022-07-16 01:13:10,Apakah Pertamina bisa menjamin kerahasiaan data masyarakat yang di unduh pada app my pertamina tersebut</t>
+  </si>
+  <si>
+    <t>,1,2022-07-16 00:58:25,Semenjak saya install MyPertamina . wah hidup saya makin bervariasi ini aplikasi benar-benar membayar tanpa iklan . mainkan terus aplikasinya agar hidup anda menjadi beban . ingat saat hidup tidak ada beban andalah yg menjadi beban . secara virtual aplikasi ini sangat virtual . semangat MyPertamina . grafis sangat lancar . mantabbbb .</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2022-08-27 14:30:40 sangat menyenangkan dengan adanya mypertamina dari pemerintah semoga lebih teratur lagi dan lebih bagus lagi agar pertamina lebih dipercaya oleh masyarakat seluruh indonesia</t>
+  </si>
+  <si>
+    <t>Pelayanan memuaskan waktu bantu bikin .aplikasi subsidi</t>
+  </si>
+  <si>
+    <t>Sudah 1 bulan belum dapat barkot hadeh....</t>
+  </si>
+  <si>
+    <t>Susah ngisinya ,,,data yang sudah diisi selalu hilang,sudah mau siap di isi data nya,, selalu saja balik ke menu awal...</t>
+  </si>
+  <si>
+    <r>
+      <t>:18:00</t>
     </r>
     <r>
       <rPr>
@@ -65,7 +870,12 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>20/12/202207:18:00</t>
+      <t>Data engga valid masak pertalite data bacanya bio solar, data base ngambil dari mana coba, parah, BUMN masak begini buat app data,,, seriusan dikit napa</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <t>:34:00</t>
     </r>
     <r>
       <rPr>
@@ -84,70 +894,21 @@
         <rFont val="Times New Roman"/>
         <family val="1"/>
       </rPr>
-      <t>Data gak valid masak pertalite data bacanya bio solar, data base ngambil dari mana coba, parah, BUMN masak gini buat app data,,, seriusan dikit napa</t>
-    </r>
-  </si>
-  <si>
-    <t>Log-in password lelet minta ampun, aplikasi error kok dipasang, sinyal full bisa mendadak lemot</t>
-  </si>
-  <si>
-    <r>
-      <t>Syatary Alubie1</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>19/12/202202:34:00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Sistem cacad, udah daftar tapi kode qr tidak muncul muncul, sudah 14 hari nunggu data masih belum terverifikasi</t>
-    </r>
-  </si>
-  <si>
-    <t>Ribet untuk pengguna yang tidak memakai handphone android</t>
-  </si>
-  <si>
-    <t>Ngaco,,nmr hp uda bnr,,pin bener dikatain salah terus,,waduh,,,</t>
-  </si>
-  <si>
-    <t>Saya dan jutaan org lainnya menginstal ap ini krn terpaksa..trimakasih</t>
-  </si>
-  <si>
-    <t>Sudah daftar dan sudah isi data lengkap. Katanya akan di verifikasi paling lama 7 hari... Tp keyataanya SDH sebulan lebih masih belum diverifikasi juga.. dan blm terdaftar... Gimana...</t>
-  </si>
-  <si>
-    <r>
-      <t>Saya sdh mendaftar di my pertamina tapi pengiriman no pin nya yg 6 digit blm di kirim"bagaimana yaa?saya kasih bintang 2dl kalau sdh dpt baru saya kasih bintang5</t>
+      <t>Sistem cacat, udah daftar tapi kode qr tidak muncul muncul, sudah 14 hari nunggu data masih belum terverifikasi</t>
+    </r>
+  </si>
+  <si>
+    <t>Ngaco,,nomor hp sudah benar,,pin benar dikatain salah terus,,waduh,,,</t>
+  </si>
+  <si>
+    <t>Saya dan jutaan orang lainnya menginstal ap ini karen terpaksa..trimakasih</t>
+  </si>
+  <si>
+    <t>Sudah daftar dan sudah isi data lengkap. Katanya akan di verifikasi paling lama 7 hari... Tapi keyataanya SuDaH sebulan lebih masih belum diverifikasi juga.. dan belum terdaftar... baGaimana...</t>
+  </si>
+  <si>
+    <r>
+      <t>Saya sudah mendaftar di my pertamina tapi pengiriman no pin nya yg 6 digit belum di kirim"bagaimana yaa?saya kasih bintang 2 dulu kalau sudah dapat baru saya kasih bintang5</t>
     </r>
     <r>
       <rPr>
@@ -160,14 +921,14 @@
     </r>
   </si>
   <si>
-    <t>aya kecewa dengan pelayanan dari pihak Pertamina orang membeli membawa tangki besar di layanin sedangkan yg membawa kendaraan biasa yg belinya non subsidi tidak kecewa berat saya</t>
-  </si>
-  <si>
-    <t>Susah banget daftar nya pake harus npwp lah makin sini makin ribet aja,kalo emang semua nya harus pake aplikasi ini permudah dong daftar nya aing jdi lieur meli solar ge hese ,, tambah deui daftar na gagal wae</t>
-  </si>
-  <si>
-    <r>
-      <t>Sangat mempersulit sekali coba yg mau beli solar lihat di lapangan</t>
+    <t>saya kecewa dengan pelayanan dari pihak Pertamina orang membeli membawa tangki besar di layanin sedangkan yang membawa kendaraan biasa yang belinya non subsidi tidak kecewa berat saya</t>
+  </si>
+  <si>
+    <t>Susah banget daftar nya pake harus npwp lah makin sini makin ribet aja,kalo emang semua nya harus pake aplikasi ini permudah dong daftar nya aing jadi lieur beli solar  ,, tambah daftar na gagal terus</t>
+  </si>
+  <si>
+    <r>
+      <t>Sangat mempersulit sekali coba yang mau beli solar lihat di lapangan</t>
     </r>
     <r>
       <rPr>
@@ -180,74 +941,41 @@
     </r>
   </si>
   <si>
-    <t>PT pertamina memutus rejeki orang eceran minyak, mikir mikir dulu lah sebelum buat aplikasi,</t>
-  </si>
-  <si>
-    <t>Sudah daftar dari aplikasi pas mau login lewat web gak bisa, daftar ulang lewat web gak bisa jg karna nik sdh terpakai.</t>
-  </si>
-  <si>
-    <t>Makin canggih mkn susah rakyat dibuaty.....ap nant beli nasi bungkus juga hrs daftar kk juga..beli nasi hrs dftr riwat hidup capekk</t>
-  </si>
-  <si>
-    <t>Sudah daftar dan berhasil registrasi. Tapi tidak bisa masuk, jaringan bagus tetap tidak bisa masuk. OS android 10 masih tidak bisa masuk. Jadi gimana ini solusinya</t>
-  </si>
-  <si>
-    <t>Aplikasi yang mempersulit hidup rakyat jelata</t>
-  </si>
-  <si>
-    <t>ketika lupa pasword masuk ke hal utama tidak bisa ganti pasword, masih banyak yang perlu d perbaiki,</t>
-  </si>
-  <si>
-    <t>Baik dilaksanakan dgn caraini, tetapi sulit untuk mencapai tujuan kesuksesan bagi rakyat biasa,</t>
-  </si>
-  <si>
-    <t>App ga jelas daftar aja pas mau Nerima kode otp aja balik lagi ke menu awal</t>
-  </si>
-  <si>
-    <t>Padahal buka kamera buat foto stnk eh webnya malah ngerefresh sendiri. Isi data lagi dr awal. Bisa kagak bikin web llol?</t>
-  </si>
-  <si>
-    <t>Beberapa menu aplikasi sering error, tidak ada fitur auto save, semoga hari mu suram</t>
-  </si>
-  <si>
-    <t>Sangat merepotkan masyarakat aplikasibodoh sekali gak jelas ajg!!!!!!!</t>
-  </si>
-  <si>
-    <t>Hancur parah. Ringsek. Nyungsep..Ngabisin kuota aja</t>
-  </si>
-  <si>
-    <t>Tidak membantu,malah menmbah susah</t>
-  </si>
-  <si>
-    <t>Yg buat ajg nyusahin masyarakat pribumi nutup banyak rezeki orang lain mereka GK tw apa dengan kebijakan kek gini banyak Abang Abang ojol kesusahan keluarga mereka menunggu di rumah uang sekolah anak dan lain lain presiden diam doang liat ini ga guna banget</t>
-  </si>
-  <si>
-    <t>Aplikasinya sh bagus cuma ada bug dan loadingnya lama , mungkin dapat di perbaiki kembali …..</t>
-  </si>
-  <si>
-    <t>Enak ya jadi penguasa bikin aturan semaunya,rakyat sudah pusing di tambah pusing lagi..ingat gajimu dari rakyat,,dzolim</t>
-  </si>
-  <si>
-    <t>Gimana nih keterangan maxsimal 2 mb tapi yg di upload 1,5mb trus ada peringatan melebihi kapasitas, sumpah aneh,</t>
-  </si>
-  <si>
-    <t>Aplikasi mengada-ada, nyusahin masyarakat kelas bawah, subsidi itu untuk RAKYAT KELAS BAWAH dimana mereka kebanyakan TIDAK PUNYA ANDROID</t>
-  </si>
-  <si>
-    <t>a sampe 20 kali mendaftar tapi tidak juga bisa terdaftar, entah apa yg salah yg daftarkan petugas pertamina tapi dia gak tau dimana salahnya, sunggu aneh</t>
-  </si>
-  <si>
-    <t>Mau daftar program subsidi tepat trus isi biodata pribadi mau kehalaman selanjutnya tidak bisa sudah daftar ke aplikasinya maupun websitenya tetap tidak bisa ke halaman selanjutnya</t>
-  </si>
-  <si>
-    <t>Di unduh sudah.. Registrasi angele pol²an Klo lom bisa di pake ni aplikasi jgn suruh dulu org² download Ngeselin.</t>
-  </si>
-  <si>
-    <t>Hapus aja aplikasi ini gak bisa di pakai terus di spbu rawa buntu 3515309 buat menejemen spbu rawa buntu jangan alesan terus . Klw pake my pertamina</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Lumayan bagus , di percepat aja proses penggunaan apk nya jangan lemot karena kita lagi di spbu </t>
+    <t>Sudah daftar dari aplikasi pas mau login lewat web gak bisa, daftar ulang lewat web engg bisa juga karna nik sudah terpakai.</t>
+  </si>
+  <si>
+    <t>Makin canggih makin susah rakyat dibuaty.....ap nant beli nasi bungkus juga harus daftar kk juga..beli nasi harus daftar riwat hidup capekk</t>
+  </si>
+  <si>
+    <t>ketika lupa pasword masuk ke hal utama tidak bisa ganti pasword, masih banyak yang perlu di perbaiki,</t>
+  </si>
+  <si>
+    <t>App engga jelas daftar saja pas mau Nerima kode otp saja balik lagi ke menu awal</t>
+  </si>
+  <si>
+    <t>Padahal buka kamera buat foto stnk eh webnya malah ngerefresh sendiri. Isi data lagi dari awal. Bisa kagak bikin web llol?</t>
+  </si>
+  <si>
+    <t>Sangat merepotkan masyarakat aplikasi bodoh sekali tidak jelas ajg!!!!!!!</t>
+  </si>
+  <si>
+    <t>Yang buat anjing nyusahin masyarakat pribumi nutup banyak rezeki orang lain mereka engga tau apa dengan kebijakan kaya gini banyak Abang-Abang ojol kesusahan keluarga mereka menunggu di rumah uang sekolah anak dan lain-lain presiden diam doang liat ini engga guna banget</t>
+  </si>
+  <si>
+    <t>Aplikasinya sih bagus cuma ada bug dan loadingnya lama , mungkin dapat di perbaiki kembali …..</t>
+  </si>
+  <si>
+    <t>Setelah hampir sehari mengisi data diri,di subsidi tepat sasaran,pilihan simpan dn selanjutnya tidak berfungsi .tolong di perbaiki!</t>
+  </si>
+  <si>
+    <t>Downlot cuma buat kasih bintang 1 aja. Langsung uninstal. hIdup ribet enega usah di bikin mkin ribet</t>
+  </si>
+  <si>
+    <t>Metode pmbayaran yang di pkai mnggunakan linkaja, tapi tidak bisa mnghubungkan akun linkaja, aneh...aplikasi apaan begini</t>
+  </si>
+  <si>
+    <r>
+      <t>Setiap login nik yang diinput tidak dikenal</t>
     </r>
     <r>
       <rPr>
@@ -256,351 +984,24 @@
         <rFont val="Segoe UI Emoji"/>
         <family val="2"/>
       </rPr>
-      <t>😁</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Harus di daftarkan oleh petugas spbu, daftar sendiri katanya gak bisa atau sangat sulit... Begitu kata petugas spbu. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>😴</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t>Susah banget daftar nya gila,jaringan gua bagus² gini malah lemot di apk nya heran</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>😑</t>
-    </r>
-  </si>
-  <si>
-    <t>Sebenarnya sangat di butuhkan tapi ribet kalau mau daftar sudah berkali2 coba di websitenya tetap aja gak bisa memang parah pelayannya, padahal di wajibkan pakai, tapi giliran mau daftar bikin susah payah</t>
-  </si>
-  <si>
-    <t>Mantap aplikasi nya tpi seharusnya Ada komentar tentang SPBU pengisian nya nilai dan buruk SPBU di lapangan</t>
-  </si>
-  <si>
-    <t>Parah untuk pendaftaran BBM subsidi, sistem selalu gagal, ketika menghubungi call center selalu sibuk, padahal telpenggunakan pulsa pribadi, .</t>
-  </si>
-  <si>
-    <t>plikasi jelek sangat membingungkan</t>
-  </si>
-  <si>
-    <t>Aplikasi gajelss, buat mempersulit masyarakat, barang siapa yang mempersuliat urusan orang lain, maka hidup nya akan di persulit oleh allah swt</t>
-  </si>
-  <si>
-    <t>Jelek berusaha daftar tapi link hilang 2 terus.bikin darah tinggi</t>
-  </si>
-  <si>
-    <t>Saat masuk pada hkaman qr barcode selalu possward tidak sesuai padahal sudah sesuai sama pendaftaran awal</t>
-  </si>
-  <si>
-    <t>Bikin ribet doang ujung ujungnya BBM naik</t>
-  </si>
-  <si>
-    <t>Meresahkan rakyat yang sudah lansia</t>
-  </si>
-  <si>
-    <t>Kita lihat aja dulu, apa alasan pertamina harus pakai aplikasi utk isi BBM</t>
-  </si>
-  <si>
-    <t>Alhamdulillah dgn aplikasi mypertamina,dpt mendptkan bbm bersubsidi dgn tepat</t>
-  </si>
-  <si>
-    <t>Petinggi yang berbuat rakyat yang bertanggung jawab.. ekonomi rakyat kecil yg awam gak bisa berkembang dgn di persulitnya BBM.</t>
-  </si>
-  <si>
-    <t>Bad banget, buat ngisi daftar subsidi balik balik sendiri</t>
-  </si>
-  <si>
-    <t>ngk jelas, udah daftar d website nya, eh malah mau login pw nya salah mulu. . giliran mau d ganti malah email nya ngk masuk"</t>
-  </si>
-  <si>
-    <t>Maksud memudahkan rakyat, semoga maksud itu tercapai..</t>
-  </si>
-  <si>
-    <t>gimana ya bos caranya habis masukin nik trus pasword munculnya gitu gitu aja</t>
-  </si>
-  <si>
-    <t>Selalu dipaksakan..... Dari awal sampe sekarang utk daftar kendaraan g bisa app rongsok</t>
-  </si>
-  <si>
-    <t>Sungguh menyusakan dan tidak efektif.apa lagi buat kita yang di daerah papua . aplikasi nya sangan tidak optimal...dan tidak bisa si daftar</t>
-  </si>
-  <si>
-    <t>Bodoh banget ayowadah pembayaran diperluas lgi,tdk semu customer memiliki hp android dg kapasitas yg baik. Blm lagi harus memerbarui versinya stiap masanya. Inovasi d era berkembangan digitalnya dpt, tp Lebih merakyaaat laaaah. Di indonesia masih banyak wong cilik.</t>
-  </si>
-  <si>
-    <t>Saya udah login tapi beberapa hari kemhdian kok login an saya g bisa lagi ya</t>
-  </si>
-  <si>
-    <t>Saya kasih 2 bintang saja Masa sampai sekrang mendatar pengguna Bio solar bersubsidi erorr trus ribet banget bisa gx bikin aplikasi bodh</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mempersulit dan meribetkan yg sudah mudah </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🤭</t>
-    </r>
-  </si>
-  <si>
-    <t>Untuk mendaftar program subsidi tepat...susah, selalu logout sendiri sangat bikin susah rakyat!!!!!!!</t>
-  </si>
-  <si>
-    <t>Duh udah daftar cari yg bisa spbu gak suport smua. My pertamina. Sayang udah ngisi saldo kaga kepake. Aturan mah suportin dulu semua spbu baru bikin aplikasi.</t>
-  </si>
-  <si>
-    <t>Kenapa subsidi jikalau dipaksa harus membeli nonsubsidi? Antrian sekarang semakin panjang, alasan bangkrut padahal gak ada saingan.tidak berlaku bodoh</t>
-  </si>
-  <si>
-    <t>Di permudah karena masih banyak yang belum tahu</t>
-  </si>
-  <si>
-    <r>
-      <t>Aplikasi yang sangat berguna bagi masyarakat banyak kususnya para petani Dan nelayan buat pembelian bahan bakar solar dan pertalit buat mesin desel sawah dan buat bahan bakar mesin perahu</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>😊🥰</t>
-    </r>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Sungguh bagus dan bermanfaat...makasih my Pertamina </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>👍👍👍</t>
-    </r>
-  </si>
-  <si>
-    <t>Apk busuk skali buat daftar aja susah. Terus bagaimana seharusnya...bikin ribet orang aja...beli BBM aja pake aplikasi...bikin ribet bikin macet nantinya hadeh...ada2 aja ini aturan</t>
-  </si>
-  <si>
-    <t>Pendaftaran di aplikasi ini ditolak ikarena nama kelurahan TIDAK TERISI, dikarenakan pada option KELURAHAN TIDAK TERDAFTAR. Adapun nama kelurahan yang dimaksud/tidak ada optionnya adalah Kelurahan PESU Kec. Wedi, Kab. Klaten, Prov.Jateng</t>
-  </si>
-  <si>
-    <t>Menggunakan aplikasi MyPertamina sangat lah praktis dan tdk ribet.</t>
-  </si>
-  <si>
-    <t>Wow sangat bermaanfaat sekali bagi masyarakat lebih efisian sekali……</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Biasanya aplikasi untuk memudahkan, ini malah nyusahin </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🤬</t>
-    </r>
-  </si>
-  <si>
-    <t>Di spbu ga bisa pakai hp. Ehhh bikin riwehh baeeeeee</t>
-  </si>
-  <si>
-    <t>Hari ini sebagian dikota Banjarbaru diberlakukan mypertamina sangat lah mudah pengisiannya di SPBU .tidak dikuasi oleh pelangsiran lagi singga anggutan umum bisa ngisi dengan mudah pake aplikasi mypertamina.kami ucapan kan terimakasih kepada pemerintah sudah memberlakukan mudah mudahan minyak subsidi tepat sasaran sebagai mana harapan pemerintah</t>
-  </si>
-  <si>
-    <t>Kasih 1 dulu,biar semangat update videonya biar makin kocak,kalau menurutsaya tambahin dong efek recallnya sama edit video gamenya..</t>
-  </si>
-  <si>
-    <t>Semoga menjadi aplikasi terbaik</t>
-  </si>
-  <si>
-    <t>Kalo beli bmm di bus simulator harus pakai Mypertamina dulu</t>
-  </si>
-  <si>
-    <t>Ini gak bisa konekin Link Aja. Udah 2 bulan masa gak beres2 masalahnya</t>
-  </si>
-  <si>
-    <t>Bisa gak ya pembayarannya jangan paki link aja? Pake kartu debit kek..gak semua org punya dompet digital...dan gak semua orang hp nya punyab kapasitas mumpuni untuk menyimpan berbagai aplikasi..</t>
-  </si>
-  <si>
-    <t>Kira kira ada ga ya penilaian minus lima? Kebijakan bodoh dengan aplikasi bodoh. Beli gas dan BBM aja ribet. Tapi ya maklum otak mereka prinsipnya kalau bisa dipersulit kenapa harus dipermudah?</t>
-  </si>
-  <si>
-    <t>Beli bensin pakai apk. Daftar nya di apk aja susah nya minta ampun.</t>
-  </si>
-  <si>
-    <t>pload data sampai 30 menit gak selesai. Untuk yang mau daftar subsidi tepat, siapin KTP, STNK. Banyak data yang diminta. Perbaiki server datanya. Masak perusahaan Forbes 500 upload data 30 mnt gak selesai.</t>
-  </si>
-  <si>
-    <r>
-      <t>Aplikasi ngk jelas. SDH memasuka data,foto dsb. Sdh nyampe foto2 STNK sama kendaraan. Pas klik kembali lngs balik ke beranda. Padahal belum selesai Ini bagaimana sihhh. Bikin repoot aja.</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>👎👎</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> Sdh bolak balik nyoba Kya gitu terus. Payaah</t>
-    </r>
-  </si>
-  <si>
-    <t>Sudah daftar subsidi tepat dari pertama kali, tpi sampai sekarang ga bisa d claim karena password salah, udah reset pass tpi ga ada email yg masuk, daftar lg juga ga bisa! Padahal mobil 1000cc.. Komplain ke cs ga ada tanggapan!! Subsidi tepat mungkin hanya wacana menaikkan harga bbm biar masyarakat g gaduh nantinya!</t>
-  </si>
-  <si>
-    <t>Merepotkan bapak saya, yg mobilnya calya, itupun dibuat angkut kelapa (kulakan). Btw bapak saya cuma jual kelapa di pasar di bangkalan madura. Bapak gaptek. Sedang beli bengsin harus pakai ini kalau kulakan kelapa di surabaya. Bener bener repot aku ngajarinnya</t>
-  </si>
-  <si>
-    <t>Aplikasi ribet ,dikira orang" awam bisa pake aplikasi ini ,udah idup sulit dibikin tabah sulit aja ,kasian mak gw noh mau beli bensin aja suruh mikir keras buat belajar ginian</t>
-  </si>
-  <si>
-    <t>Prnh nukar point dgn jaket+replika SPBU dan replika truk Tanki tapi g di kirim</t>
-  </si>
-  <si>
-    <t>Aplikasi tidak pro rakyat, gimana rakyat kecil yg tidak punya android?</t>
-  </si>
-  <si>
-    <t>Kasi bintang 1 dulu. Aplikasi plat merah buruk dan memaksa</t>
-  </si>
-  <si>
-    <t>Aplikasinya berat bukanya, tdk smua android suport</t>
-  </si>
-  <si>
-    <t>Padahal sudah beli skin tapi tidak masuk". Hmm aplikasinya sih bagus tapi ya gtu sudah beli tapi tidak di tanggapi. Saran juga natalia jgan hilang" gitu dong kan susah untuk nge hitnya. Masa selesai mukul langsung hilang</t>
-  </si>
-  <si>
-    <t>BBM susah daftar data sudah lengkap juga masih susah udah berulang ulang tapi ga bisa daftar juga Sebenarnya mau nya pemerintah itu gimana yah kok makin mempersulit begini</t>
-  </si>
-  <si>
-    <t>tadinya app ini bagus smpe mas² operator nosel bilang "sudah tdk ad lagi jalur my pertamina" harus ikut antrian panjang... kecewa</t>
-  </si>
-  <si>
-    <t>Belum bisa beli pertalite untuk motor disemua spbu pertamina Dan yang biasanya bisa, sekarang malah jadi gak bisa, kata petugasnya hanya untuk mobil yang diprogramkan subsidi saja yang bisa</t>
-  </si>
-  <si>
-    <t>Aplikasi ndk guna bikin bingung masyarakat.klu naik ndk USA membingungkan.pikirin rakyat ya pejabat</t>
-  </si>
-  <si>
-    <t>Untuk aplikasi nya sudah bagus cuman grafik nya agak burik sama sama</t>
-  </si>
-  <si>
-    <t>Untuk pihak program MyPertamina saya minta tolong untuk proses verifikasi setelah pendaftaran dilakukan agar secepatnya diterima,agar kami bisa sesegera mungkn mendapatkan Kode QR (Barcode). Hanya karna blm diverifikasi sampai saat ini saya sudah 3 hari kesulitan mendapatkan BBM.,jadi saya mnta tolong bantu kami dengan cara mempercepat proses pengambilan barcodw untuk pendaftar baru.temksh ..</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Suruh pake aplikasi tapi pembayaran hanya terbatas di satu pembayaran aja, kalo udh wajib harusnya metode pembayaran ya bisa semua tetapi sudah sangat membantu </t>
-  </si>
-  <si>
-    <t>Buruk sekali...tidak bisa dapat melanjutkan perintah setelah tersimpan data pribadi...gimana nih... kejam</t>
-  </si>
-  <si>
-    <t>Aplikasi tolol tanggal lahir gw salah tauan siapa gw apa lo... Beli bensin aja ribet... Naikin terus harga nya</t>
-  </si>
-  <si>
-    <t>INI MAH MEMPERSULIT BUKAN MEMPERMUDAH.BANGSATTTTT!!!!!!!!!</t>
-  </si>
-  <si>
-    <t>Mohon kepada owner aplikasi, ditempat saya sudah di perlakukan aplikasi my Pertamina.. dan saya sudah download dan mau daftar sudah mengisi data diri lengkap saya pencet selanjutnya tidak bisa .. mohon kepada owner aplikasi nya . Ini kenapa ya?</t>
-  </si>
-  <si>
-    <t>banyak spbu Pertamina yang belum menggunakan app nya.</t>
-  </si>
-  <si>
-    <t>INI sangat cocok untuk pembelian BBM</t>
-  </si>
-  <si>
-    <t>Aplikasi N**ntot! Mempersusah untuk isi bensin!</t>
-  </si>
-  <si>
-    <t>Aplikasi susah dan mempersulit. Mohon pertamina kalau membuat aplikasi di uji coba dulu bisa suport gak. Jangan selalu salahkan pengguna atau masyarakat.</t>
-  </si>
-  <si>
-    <t>Mau daftarin kendaran aplikasi kluar sendirinya wkwk Gmnain mau ngikutin aturan coba aplikasinya gini Hp ram 4 gb Internal msih banyak kosong</t>
-  </si>
-  <si>
-    <t>Disaat edit data, password claimnya tdk bs di claim, di email di verifikaai tetapi tdk bisa confirm new password claim. Tdk ada popup ketikan yg sebelumnya</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">mau claim QR code susah nya kaya nyari keadilan di negeri ini. bukannya di bikin mudah, malah di bikin ribet </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🖕🖕🖕🖕</t>
-    </r>
-  </si>
-  <si>
-    <t>Yang penting ketersediaan BBM tetap terjaga...dan aplikasi onlini ini bisa membantu PD saat mengisi d spbu..bukan hanya sekedar aplikasi saja</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Mengikuti peraturan yang berada saat ini </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>😎</t>
-    </r>
-  </si>
-  <si>
-    <t>Dengan Mypertamina kita jd mudah untuk membeli pertalite</t>
-  </si>
-  <si>
-    <t>Efektif sih untuk yang mudqh milenia kalqu untuk orang tua kita yang ngga sekolah susah bangsatt!!!!!!!!!!</t>
-  </si>
-  <si>
-    <t>Sangat buruk.pelayan tidak baik. Beli solar di susah2. Beli pertalit di susah2. Beli pertama k di susah2. Dasar orang2 gak per akhlak.saya sumpahin lo beserta anak turun lo bakal kena karmanya</t>
-  </si>
-  <si>
-    <r>
-      <t>Gagal verifikasi katanya suruh ganti foto lain. Tapi udah d ganti dan ternyata tombol update data g fungsi</t>
+      <t>🤷</t>
+    </r>
+  </si>
+  <si>
+    <t>Mantap engga bisa nyeleweng lagi</t>
+  </si>
+  <si>
+    <t>bikin emosi saja kode otp ga masuk² !!!!!!!!!!!!! aplikasi jelek banget kalau engga disruh pake aplikasi ini buat isi bensin saya juga males install</t>
+  </si>
+  <si>
+    <t>Saya optimis kita semua bisa membenahi negeri ini dengan kemauan yang tinggi</t>
+  </si>
+  <si>
+    <t>kita semua harus percaya dan bisa membenahi negeri ini dengan kemauan yang tinggi</t>
+  </si>
+  <si>
+    <r>
+      <t>Gagal verifikasi katanya suruh ganti foto lain. Tapi udah di ganti dan ternyata tombol update data engga fungsi</t>
     </r>
     <r>
       <rPr>
@@ -613,467 +1014,28 @@
     </r>
   </si>
   <si>
-    <t>kita semua harus percaya dan bisa membenahi negeri ini dengan kemauan yg tinggi</t>
-  </si>
-  <si>
-    <t>Saya optimis kita semua bisa membenahi negeri ini dengan kemauan yg tinggi</t>
-  </si>
-  <si>
-    <t>Rumit sangat tidak membantu, metode klaim pembayaran cuma pakai link aja, seharusnya ditambahkan aplikasi lainnya jangan link aja, saya curiga ada permainan apa disini, meribetkan rakyat kecil yg tidak paham dan tidak bisa menggunakan aplikasi, nanti subsidibya cuma untuk org yg berduit saja, ribet untuk semuanya</t>
-  </si>
-  <si>
-    <t>Dafar My Pertamina. Caranya Mendapatkan aplikasi my pertamima</t>
-  </si>
-  <si>
-    <t>Aplikasinya sudah bagus tapi kebijakannya konyol jadi bintang 1.</t>
-  </si>
-  <si>
-    <t>bikin emosi aja kode otp ga masuk² !!!!!!!!!!!!! aplikasi jelek banget kalau ga disruh pake aplikasi ini buat isi bensin saya juga males install</t>
-  </si>
-  <si>
-    <t>Mantap ngak bisa nyeleweng lagi</t>
-  </si>
-  <si>
-    <r>
-      <t>Setiap login nik yg diinput tidak dikenal</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🤷</t>
-    </r>
-  </si>
-  <si>
-    <t>Metode pmbayaran yg d pkai mnggunakan linkaja, tp tidak bsa mnghubungkan akun linkaja, aneh...aplikasi apaan bgni</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">Kasih 2 </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>🌟🌟</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t xml:space="preserve"> dulu soalnya belum tahu manfaat ke depannya bagaimana</t>
-    </r>
-  </si>
-  <si>
-    <t>Donlot cuma buat kasih bintang 1 aja. Langsung uninstal. Idup ribet ga usah d bikin mkin ribet</t>
-  </si>
-  <si>
-    <t>Setelah hampir sehari mengisi data diri,di subsidi tepat sasaran,pilihan simpan dn selanjutnya tdk berfungsi.tolong di perbaiki!</t>
-  </si>
-  <si>
-    <r>
-      <t>Dengan aplikasi MyPertamina</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <color theme="1"/>
-        <rFont val="Segoe UI Emoji"/>
-        <family val="2"/>
-      </rPr>
-      <t>👍👍</t>
-    </r>
-  </si>
-  <si>
-    <t>Masih ada banyak kekurangan / ada banyak sekali bug dan mempersulit bagi pengguna aplikasi nya tolol yang bikin</t>
-  </si>
-  <si>
-    <t>Tolong di batasin donk pembelian pertalite yg menggunakan kapasitas besar</t>
-  </si>
-  <si>
-    <t>Ga semua konsumen punya smartphone....beli bbm kok ribet....infrastruktur jaringan internet juga belum merata..... Negara seharusnya mengayomi dan menjamin hidup rakyatnya, bukanya malah berbisnis dengan rakyat.</t>
-  </si>
-  <si>
-    <t>text</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 2022-08-27 14:30:40 sangat menyenangkan dengan adanya mypertamina dari pemerintah se moga lebih teratur lagi dan lebih bagus lagi agar pertamina lebih dipercaya oleh masyarakat seluruh indonesia</t>
-  </si>
-  <si>
-    <t>,1,2022-07-15 23:29:56,"Semoga aplikasinya cepat diperbaiki, karena begitu banyak masalah saat menggunakan aplikasi ini, setidaknya jangan membuat kami tambah susah,karena kami udah sangat susah."</t>
-  </si>
-  <si>
-    <t>,1,2022-07-16 00:58:25,Semenjak saya install MyPertamina . wah hidup saya makin bervariasi ini aplikasi benar benar membayar tanpa iklan . mainkan terus aplikasinya agar hidup anda menjadi beban . ingat saat hidup tidak ada beban andalah yg menjadi beban . secara virtual aplikasi ini sangat virtual . semangat MyPertamina . gtafis sangat lancar . mantabbbb .</t>
-  </si>
-  <si>
-    <t>,1,2022-07-16 01:13:10,Apakah Pertamina bisa menjamin kerahasiaan data masyarakat yg di unduh pd app my pertamina tsb</t>
-  </si>
-  <si>
-    <t>,5,2022-07-16 04:16:15,"Aplikasi MyPertamina wajib dimiliki untuk kemudahan transaksi pembelian BBM diseluruh IndonÃ©sia, sangat mudah mengoperasikan dan terintegrasi dengan data kita"</t>
-  </si>
-  <si>
-    <t>,5,2022-07-16 08:02:23,Bermanfaat banget kalau mau tracking pengeluaran bbm</t>
-  </si>
-  <si>
-    <t>,1,2022-07-16 08:31:23,Ribet lu isi bensin aja ribetðŸ‘Ž</t>
-  </si>
-  <si>
-    <t>,1,2022-07-16 11:41:40,Aplikasi payah...lelet...ðŸ‘ŽðŸ‘ŽðŸ‘ŽðŸ‘Ž</t>
-  </si>
-  <si>
-    <t>,1,2022-07-16 12:14:53,"selalu ditunggangi dengn kpntingan"" yg menguntungkan beberapa pihak ðŸ˜” aku menyebutnya MIRIS &amp; KONYOL"</t>
-  </si>
-  <si>
-    <t>,1,2022-07-16 14:14:19,Pertamina tolol udah tau yg isi bensin motor kebanyakan org tua lu pikir semua org tua tau apa cara makai ini apk</t>
-  </si>
-  <si>
-    <t>:06:00Daftar dan menghubungkan ke link aja cepat ga nyampe 5 menit ðŸ‘ðŸ»ðŸ‘ðŸ» semoga untuk kedepan ga ada kendala</t>
-  </si>
-  <si>
-    <t>01:59:22,aplikasi yang Sangat Merepotkan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01:57:22,Tidak Berguna Dan Sangat Merepotkan</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 02:06:11,"Awalnya terasa Ribet, Seiring Waktu Semakin Praktis, Jaya Selalu Pertamina."</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 02:24:23,Aplikasi yang sangat bagus &amp; sangat mempermudah saat bertransaksi. Terima kasih MyPertamina ðŸ‘ðŸ‘ðŸ‘</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 02:49:05,Kembali ke normal lagi tanpa aplikasi ðŸ¤²</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 04:28:31,Setelah diupdate baru bisa buka aplikasi MyPertamina. Waktu mau daftar kendaraan sesuai kemauan pemerintah tidak bisa masukan data2. Saya tambah satu bintang saja.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 05:55:27,Konfirmasi datanya lama Keburu behan bakarnya habisðŸ˜ ðŸ˜ ðŸ˜ ðŸ˜</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 07:09:09,Ø§Ù„Ø­Ù…Ø¯ Ù„Ù„Ù‡ Alhamdulillah Bagus Good</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 09:34:56,"SEMANGAAAT MY PERTAMINAAA, trus berkembaang yaðŸ¥³. Bisa yok bisa. Udh banyak yg make sistem aplikasi d beberapa tmpt tertentu contoh nya bpjs kesehatan(jkn mobil) Bpjs ketenagakerjaan(jmo mobile) dan saya pribadi merasa sangat terbantu dgn kemudahan yg d berikan jdi segala nya bisa lewat hp aj"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10:46:06,My pertamina bikin ribet menurut saya Kenapa harus pakai pertamina Bagus seperti dlu saja Harus nya indonesia Bukan masalah BBm nya yg di persulit Tapi kendaraan nya jangan setiap tahun Diproduksi tambah macet jadi nya Enak jaman dulu ga banyak kendaraan Sekarang 80% jdi rawan kecelakaan Karena kebanyakan pemotor/yg bermobil Yg masih abg atau yg sudah tua juga naik motor/mobil sendiri gimna ga habis minyak bumi Kalau kendaraan setiap tahun ditambah terus</t>
-  </si>
-  <si>
-    <t>12:26:27,"My pertamina sendiri belum siap kok. M`asak sdh ngulang 10 kali kok tetap ""ada gangguan dan tidak bisa diinput"" mbelgedes"</t>
-  </si>
-  <si>
-    <t>iya!!!!!!ðŸ‘‰ðŸ‘ŒðŸ‘‰ðŸ‘ŒðŸ‘‰ðŸ‘ŒðŸ‘‰ðŸ‘ŒðŸ’¦"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14:09:53,"buat pertamina, saya dukung program nya.. maju terus, memang mengubah kebiasaaan itu susah.. tpi nanti lama2 klo udah terbiasa juga bisa diterima"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 17:59:51,aplikasi buat susah banyak spam bug dll hadeh payah ne aplikasi.. tolong hapus saja aplikasi ini sangat tidak menolong</t>
-  </si>
-  <si>
-    <t>04:04:13,Hmmm td coba isi bensi dan bayar pakai mypertamina erorr saat mau pembayaran alhasil pakai cash...</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 23:37:52,Kebanyakan aturan ribet banget anjg bikin orang tambah susah njg!!!!!</t>
-  </si>
-  <si>
-    <t>18 00:00:11,Sangat membantu sekali karna saya dapat membeli bbm dengan mudah tanpa harus membawa uang cash..,,</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 02:40:34,"Susah diopeasikan, sering ngelag, error trs, tidak memuaskan pokoknya,"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 04:00:01,Dukung kemajuan Indonesias</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 05:01:03aplikasi my,Pertamina mantap</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 07:14:56,sudah ngisi identitas. Nggk bisa daftar2. Susah. Di suruh upload foto tp nggk bisa buat upload. Cma hitam tok di layar.. Aplikasi blm bener2 siap tp sudah di paksakan.</t>
-  </si>
-  <si>
-    <t>10:52:00Aplikasi sampah, udah terferifikasi dari bulan juli qr code dah dapet, ganti hp malah gabisa claim qr code lagi, APLIKASI SAMPAH !!!ðŸ—¿</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 08:57:00,Sudah terkonfirmasi saat claim qr code muncul belum terverifikasi gmn neh payah.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 09:12:13,Nyobain tadi bayar bensin pake app ini. Udah di isi 21 rebu. Eh pas mau bayar aplikasi nya coba lagi coba lagi Mulu. Ampe setengah jam ngotak ngatik ini aplikasi. Padahal jaringan bagus. Mana kaga bawa duit. Parah dah. Malu maluin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10:40:30,Mempersulit rakyat</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 10:54:20,Udah daftar buat kode qr udah seminggu lebih tapi gak diverifikasi</t>
-  </si>
-  <si>
-    <t>18 07:13:35,Tidak bisa login padahal udah daftat</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11:06:11,Aplikasi yg tidak perlu sangat sangat bodoh yg menyatankan aplikasi ini</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11:44:11,"Sistem apaan ini?? Yg ngasih bintang lima gak ada otak, anjg!"</t>
-  </si>
-  <si>
-    <t>1,2022-07-18 11:50:15,Mohon perbaikannya terlalu banyak bug apalagi saat bertemu tiba tiba sat set swing.... Grafis Nya mohon di tingkat kan lagi sayang banget game sebagus ini banyak bug nya....</t>
-  </si>
-  <si>
-    <t>1,2022-07-18 12:08:16,Entah ini apk buat apa gajelas</t>
-  </si>
-  <si>
-    <t>1,2022-07-18 12:12:41,Merepotkan sekali, sangat bodoh apk nyaa ajg lah…..</t>
-  </si>
-  <si>
-    <t>1,2022-07-18 12:26:18,Semoga bbm harganya turun amin</t>
-  </si>
-  <si>
-    <t>02:00Bikin ribet, mau menghubungkan ke link saja tidak bisa dengan alasan waktu habis, bikin aplikasi apa ini sangat jelek sekaliðŸ˜‘ðŸ˜‘ðŸ˜‘ðŸ˜‘</t>
-  </si>
-  <si>
-    <t>02:50:41,Bagus sekali aplikasinya sangat membantu dan lebih efektif serta efsien,……</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:02:42,Keren dan mempermudah,  inovatif salam sukses</t>
-  </si>
-  <si>
-    <t>03:07:56,Sangat memuaskan... Kedepan lebih mudah dan bermanfaat.. ðŸ‘</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:38:22,Mantapdan lebih efisen </t>
-  </si>
-  <si>
-    <t>03:40:25,Terimakasih sudah terdaftar sebagai penerima bbm bersubsididan sangat. Lah baik</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 06:16:22,"Sebenarnya tujuannnya bagus, tapi langkahnya mungkin kurang efektif, ya. My pertamina sudah bisa mengambil data ribuan kendaraan dari aplikasi transportasi, katakan kerjasama pemberian barcode. Sisanya tingal yg tidak ada aplikasi transportasi. Selain itu, masyarakat agak curiga ini aplikasi akal2an guna menaikkan aplikasi Link aja. Karena kalo mau adil semua metode pembayaran ovo, gopay dan yg lain harus bisa di integrasikan. Terima kasih semoga masukan kami bermanfaat."</t>
-  </si>
-  <si>
-    <t>10:00aplikasi yg sangat tidak berguna, membingungkan mutar muter bertele tele.</t>
-  </si>
-  <si>
-    <t>09:28:35,Tolong permudah pembayaran via gopay atau ovo....terima kasih.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12:05:12,Untuk aplikasinya udh cukup bagus ya intinya di permudah aja dalam pembayaran Pokoknya bagus lah</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:02:42,Keren inovatif salam sukses</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:07:56,Sangat memuaskan... Kedepan lebih mudah dan bermanfaat.. ðŸ‘</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:27:46,Pakai mypertamina sangat praktis.</t>
-  </si>
-  <si>
-    <t>13:00 App tsb sdh sangat mendukung transaksi non tunai, tp ada bbrp SPBU masih bayar dlu baru isi BBM, bukannya kebalikan berapa ril di Isi baru bayar, ðŸ™</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:40:25,Terimakasih sudah terdaftar sebagai penerima bbm bersubsidi. Bintang 3 dlu ya</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 04:43:53,"Niat mempermudah, tp hasilnya mempersusah masyarakat, aplikasinya tidak berbobot, di perbaikannya, dan sebagai masukan Kalau E-walet y jangan cuma satu aja donk, dan juga apakah pihak pengembangan sudah memikirkan bagai mana bagi orang-orang tua yg kurang paham pakai android, atau yg gx punya HP android... Kan jd susah, kasiahan mereka yg tidak punya android dan tidak paham android."</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 07:34:48,"Setelah sekian lama daftar baru dapat notifikasi dan QR codenya. Scara penggunaan aplikasi myPertamina dapat mudah dilakukan di kota besar. Sekarang tinggal masalah di ketersediaan pertalite-nyaðŸ˜“. Beberapa kali masuk SPBU, pertalite kosong"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 11:28:20,Kalau untuk tujuan tepat sasaran pemakai bbm subsidi sih ok. Cuma cara menggunakan agar bisa lebih di permudah</t>
-  </si>
-  <si>
-    <t>12:05:12,Untuk aplikasinya udh cukup bagus ya intinya di permudah aja dalam pembayaran Pokoknya bagus lah</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12:17:28,Mohon pihak playstore dan Stade holder terkait karena menyusahkan masyarakat kalangan bawah dan menengah dan mengajukan keberatan dengan aplikasi my Pertamina karena sistem login menggunakan nomor ponsel pengguna akun lainnya dan serta pin rekening bank ini bisa mempermudah hacker mencuri data pengguna akun lainnya di seluruh Indonesia dan menggunakan password yang belum aman dari sistem keamanan yang menjamin pengguna akun lainnya di seluruh Indonesia dan mohon diblokir aplikasi my Pertamina</t>
-  </si>
-  <si>
-    <t>21:17:00aplikasi yang sangat buruk untuk pelayanan masyarakat ,hanya untuk merubah data kendaraan saja sudah 2 hari tidak bisa diupdate!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 14:50:18,"Tidak efektif, udh jelas ada tanda hp dilarang malah main hp jadinya di spbu, ga jelas juga kegunaannya untuk apa ðŸ‘Ž"</t>
-  </si>
-  <si>
-    <t>15:02:25,Aplikasi tidak berguna babi anjing ngentod tai bangast celeh asu sia kontol anjing appk mensulitkan masyarakat bangast anjing sia anjing ngentod seng gae pekok tolol goblok lulusan tk</t>
-  </si>
-  <si>
-    <t>00:18:00Aplikasi tidak ada guna nya kebanyakan tidak bisa di gunakan seluruh pertamina..kapan di tanya pagi tidak bisa,kapan di tanya malam tidak bisa..terus kapan bisa...tolong tegas buat kebijakan nya..jangan buat kebijakan tidak tegas dan tidak bermutu.</t>
-  </si>
-  <si>
-    <t>02:29:00Aplikasi ga guna!!! Daftar susah, nelpon call center ketus, belum selesai ngomong udah di sela!! Aplikasi ga ada guna!!!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 16:27:13,Mantap sekali apknyaðŸ‘</t>
-  </si>
-  <si>
-    <t>21:42:00,BIKIN RIBET AJA PAKE APLIKASI. LEBIH ENAK BAYAR TUNAI!!! NO DEBAT!</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 22:47:41,Daftar program subsidi ga bisa terus...payah nih apk</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 01:41:42,"Pelayanan menggunakan MyPertamina selama saya pakai ini utk pengisian bensin motor di SPBU Pertamina sangatlah bagus, praktis juga pelayanan petugas SPBUnya sangat ramah sekali. Dan banyak hadiah yg bagus2 utk setiap pembelian bensin. Sudah dapet bensin ++++ dapet kupon poinnya yg bisa dtukarkan berupa hadiah yg bagus sesuai dgn poin kita. Mohon utk ditingkatkan terus pelayanan MyPertamina utk kedepannnya lebih bagus &amp; hadiahnya yg keren2.... Terima kasih ðŸ™"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 02:33:33,"Apk pembodohan, yakali disave gaisa tulisan ga ada jaringan, pencet membali juga kembali ke awal ngulang lagi dari awal sampe ngulang 5x tetep aja gaisa ckckck"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 02:54:33,"Aplikasi gak jelas,masa sinkronin ke metode pembayarannya aja gak bisa bisa..."</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 03:40:23,Aplikasi paan sih. Login g bisa daftar ga bisa. Cacat.</t>
-  </si>
-  <si>
-    <t>15:32:00Aplikasi macam apa, saya sudah daftar kemaren masak sekali update aplikasinya saya harus daftar balik. Kan taik itu. Masak barcode saya hilang di apliaksinya harus daftar kembali. Aplikasi macam apa ini</t>
-  </si>
-  <si>
-    <t>02:25:00 Bagus cara mendaftar gampang bagi yg sudah tau. cuma untuk pendaftaran diaplikasi kadang bermasalah. Alternatif lain bisa diweb SUBSIDI TEPAT. Terkadang ada Hp yg tidak support dengan aplikasinya. Untuk Edit data Lebih bagus di aplikasi karena diweb sering bug. Web hanya (untuk daftar) 1. centang 2.pilih daftar sekarang. 3.isi data pendaftaran 4.disini ukuran foto tidak boleh dari 2 MB (harus di kompres). 5.untuk kode verifikasi akan dikirim melalui email.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 04:43:25,semoga sesuai dengan tujuan bagi yang berhak mendapat subsidi bbm</t>
-  </si>
-  <si>
-    <t>04:44:18,Semoga subsidi BBM tepat sasaran</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 05:50:45,Gak guna... Unsinstall aja lah</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 06:40:46,Saya sebagai sopir angkot dan saya gaptek tehnologi dan saya secara tdk langsung di paksa harus beli hp amdroit sebagaimana fungsinya utk membeli bengsin dan saya terpaksa harus hutang demi membeli hp utk kebutuhan hidup karena anak saya 3 dan sekolah semua</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 07:02:20,"Aplikasi kayak gini mau di wajibin? Sering error pas pembayaran, gak praktis sama sekali! Perbaiki lah pembayaran harus melalui lingajah, tapi suka error."</t>
-  </si>
-  <si>
-    <t>06:02:00Jadi begini masalahnya, ketika Saya tidak membawa uang cash, maka saya sangat tergantung dengan aplikasi my pertamina. Tapi yang sangat mengecewakan adalah ketika sudah selesai isi pertamax, ternyata pembayaran menggunakan mypertamina malah gangguan. Nah ini sangat memalukan sekali….apalagi saat tidak membawa uang cash. Saya sudah berkalikali di permalukan sama aplikasi ini karena setiap akan melakukan pembayaran, selalu mengalami gangguan dan akhirnya harus ambil uang diu atm. ðŸ˜ðŸ˜µðŸ˜¡</t>
-  </si>
-  <si>
-    <t>08:51:49,"Gk boleh make hp di SPBU, tapi disuruh download aplikasi terus make si SPBU,"</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 09:03:46,"Buat kebijakan harus di pikiri sebelum di laksanakan , jgan ambil keputusan meliat dari posisi kamu berada , liat dari sekitar dan secara luas juga."</t>
-  </si>
-  <si>
-    <t>09:32:01,Ini apaan sih daftarin kendaraan capek2 di email sudah di aprov tpi login gagal mulu yg nik gak sama yg nopol gak kedaftar... Daftar lagi udah gak bsa nik terdaftar... Bukn nya bikin simple malah bikin males yg ada</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 09:34:58,APLIKASI TIDAK BERGUNA!!!!</t>
-  </si>
-  <si>
-    <t>09:35:19,Merepotkan warga desa seperti saya</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 09:38:05,Aplikasi tidak bagus. Berbelit. Aplikasi pura pura hanya untuk menutupi program yang lain</t>
-  </si>
-  <si>
-    <t>10:00:22,Aplikasi tidak layak pakai</t>
-  </si>
-  <si>
-    <t>12:40:00Untuk aplikasi sih sudah mantap...hanya saja sayangnya tidak di gunakan dengan baik oleh para SPBU,bisa di katakan untuk sekarang SPBU masih lebih suka dengan uang</t>
-  </si>
-  <si>
-    <t>10:06:38,Sangat menyenangkan tidak usah mengeluarkan uang tinggal keluarkan hp dan di tunjukkan aplikasi my pertamina sdh selesai asal saldonya cukup</t>
-  </si>
-  <si>
-    <t>10:08:01,Tidak sebagus my pertamina unlimited mode</t>
-  </si>
-  <si>
-    <t>10:14:32,"Tidak bisa tersambung, susah di pake di spbu gak boleh mainan hp"</t>
-  </si>
-  <si>
-    <t>10:22:06,"Ini sebenarnya pertamina niat gak sih bikin aplikasi, sudah berhari-hari error terus. dikasih waktu tenggang sampe 30 Juli. Perusahaan bumn besar urusan aplikasi aja sampe kaya gini banget."</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 02:51:00enak si pakai aplikasi, gk ribetÂ² bawa uang Cash, semua serba digital, tapi gk ada casehback 25%, padahal di Sticker SPBU terpampang casehback nya ðŸ˜</t>
-  </si>
-  <si>
-    <t>10:37:33,"Saat mengisi data tanggal lahir, anehnya bulan Februari tidak bisa dipilih. Saat memilih Februari, yang muncul di pengisian malah Januari. Mohon dikoreksi, terima kasih."</t>
-  </si>
-  <si>
-    <t>10:53:42,Contoh aplikasi ygmenyengsarakn rakyat</t>
-  </si>
-  <si>
-    <t>11:22:36,"Subsidi biar tepat sasaran.... Mantabs, maju terus pertamina. NKRI harga mati.."</t>
-  </si>
-  <si>
-    <t>11:34:01,Mempersulit rakyat</t>
-  </si>
-  <si>
-    <t>06:37:00Aplikasi yg buruk sekali... Foto bolak balik stnk tetap tidak terbaca.. Padahal jelas sekali fotonya.. Sehingga menghambat pendaftaran…</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 12:05:01,"Gini orang suruh pake, udah ribet, error gobblk pula, link aja juga sama gblknya bikin malu aja pas scan gagal terus aplikasi sialan"</t>
-  </si>
-  <si>
-    <t>11:46:00Susah penggunaannya. Beberapa kali mo beli bensin lewat aplikasi biar bisa dapat poin loyality susah, ditanya ke pegawainya bilangnya ini itu lah. Ga ada petunjuk yang jelas</t>
-  </si>
-  <si>
-    <t>12:22:53,"Aplikasi kurang siap masa tiap masuk aplikasi harus masukin password dulu, padahal password udah disimpan aplikasi."</t>
-  </si>
-  <si>
-    <t>12:34:03,"Aplikasi yang menyusahkan manusia Kata nya di pom bensi gk boleh main hp In kok di izin ini bukak hp? Gimana kalau pom itu kebakar oleh kita bukak hp emang ad garansi kah misal nya kami kenapa"" oleh ledakan minyak?"</t>
-  </si>
-  <si>
-    <r>
-      <t>03:48:00</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="12"/>
-        <rFont val="Times New Roman"/>
-        <family val="1"/>
-      </rPr>
-      <t>Daftarnya ribet, iklan diawal sangat mengganggu, ui/ux tidak responsif</t>
-    </r>
-  </si>
-  <si>
-    <t>01:03:22,Aplikasi buruk sekali</t>
-  </si>
-  <si>
-    <t>01:01:56,Udah susah jadi tambah susah</t>
-  </si>
-  <si>
-    <t>00:58:25,Semenjak saya install MyPertamina . wah hidup saya makin bervariasi ini aplikasi benar benar membayar tanpa iklan . mainkan terus aplikasinya agar hidup anda menjadi beban . ingat saat hidup tidak ada beban andalah yg menjadi beban . secara virtual aplikasi ini sangat virtual . semangat MyPertamina . gtafis sangat lancar . mantabbbb .</t>
-  </si>
-  <si>
-    <t>08:26:00Kok payah x dapat email nya otp nya . . . Bantu lah . Lalap sedikit 2 nik salah n pasword salah apa nya ni app ?</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00:05:01,Mempersulit hidup orang yang udah sulit. Harus dihubungkan dengan link aja. Udah tahu gak semua HP memdai.</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> 00:00:53,"Maaf kasih 1 bntng karna ga epektif, malah tambah ribet. Mau daftar susah masuk."</t>
-  </si>
-  <si>
-    <t>23:45:23,Selevel negara kok g mampu bikin aplikasi yg baik. Udah dftr ulang2 tp g bisa login krn no HP/PIN salah. Pdhl sdh masukkan dgn benar. Bisa g sih negara g persulit rakyat sendiri?</t>
-  </si>
-  <si>
-    <t>23:41:43,Ntah laah susah di jelaskan....ribeet…</t>
-  </si>
-  <si>
-    <t>23:31:43,Aplikasi apa ini nik tidak terbaca</t>
-  </si>
-  <si>
-    <t>23:29:56,"Semoga aplikasinya cepat diperbaiki, karena begitu banyak masalah saat menggunakan aplikasi ini aplikasi ini, setidaknya jangan membuat kami tambah susah,karena kami udah sangat susah."</t>
+    <t>Sangat buruk.pelayan tidak baik. Beli solar di susah2. Beli pertalit di susah2. Beli pertamax di susah2. Dasar orang2 engga per akhlak.saya sumpahin kamu beserta anak turun kamu bakal kena karmanya</t>
+  </si>
+  <si>
+    <t>Efektif sih untuk yang mudqh milenia kalau untuk orang tua kita yang ngga sekolah susah bangsatt!!!!!!!!!!</t>
+  </si>
+  <si>
+    <t>Dengan Mypertamina kita jadi mudah untuk membeli pertalite</t>
+  </si>
+  <si>
+    <t>Yang penting ketersediaan BBM tetap terjaga...dan aplikasi onlini ini bisa membantu PaDa saat mengisi di spbu..bukan hanya sekedar aplikasi saja</t>
+  </si>
+  <si>
+    <t>Disaat edit data, password claimnya tidak bisa di claim, di email di verifikaai tetapi tidak bisa confirm new password claim. Tidak ada popup ketikan yang sebelumnya</t>
+  </si>
+  <si>
+    <t>Mau daftarin kendaran aplikasi keluar sendirinya wkwk bagaimana mau mengikuti aturan coba aplikasinya begini Hp ram 4 gb Internal masih banyak kosong</t>
+  </si>
+  <si>
+    <t>Aplikasi susah dan mempersulit. Mohon pertamina kalau membuat aplikasi di uji coba dulu bisa suport engga.  Jangan selalu salahkan pengguna atau masyarakat.</t>
+  </si>
+  <si>
+    <t>banyak spbu Pertamina yang belum menggunakan aplikasi nya.</t>
   </si>
 </sst>
 </file>
@@ -1524,18 +1486,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0B7D317-0B74-44A0-92B9-2672DAB14D47}">
   <dimension ref="A1:B251"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="148" zoomScaleNormal="148" workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" topLeftCell="A222" zoomScale="91" zoomScaleNormal="91" workbookViewId="0">
+      <selection activeCell="A222" sqref="A222"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="162.7109375" customWidth="1"/>
+    <col min="1" max="1" width="179" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
-        <v>134</v>
+        <v>96</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -1543,7 +1505,7 @@
     </row>
     <row r="2" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
-        <v>251</v>
+        <v>206</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -1551,7 +1513,7 @@
     </row>
     <row r="3" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="4" t="s">
-        <v>250</v>
+        <v>166</v>
       </c>
       <c r="B3" s="1">
         <v>1</v>
@@ -1559,7 +1521,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>249</v>
+        <v>167</v>
       </c>
       <c r="B4" s="1">
         <v>0</v>
@@ -1567,7 +1529,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>248</v>
+        <v>168</v>
       </c>
       <c r="B5" s="2">
         <v>0</v>
@@ -1575,7 +1537,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="5" t="s">
-        <v>247</v>
+        <v>170</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1583,7 +1545,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="5" t="s">
-        <v>246</v>
+        <v>165</v>
       </c>
       <c r="B7" s="1">
         <v>0</v>
@@ -1591,7 +1553,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>245</v>
+        <v>164</v>
       </c>
       <c r="B8" s="1">
         <v>0</v>
@@ -1599,7 +1561,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="5" t="s">
-        <v>244</v>
+        <v>163</v>
       </c>
       <c r="B9" s="2">
         <v>1</v>
@@ -1607,7 +1569,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="5" t="s">
-        <v>243</v>
+        <v>162</v>
       </c>
       <c r="B10" s="2">
         <v>0</v>
@@ -1615,7 +1577,7 @@
     </row>
     <row r="11" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>242</v>
+        <v>161</v>
       </c>
       <c r="B11" s="2">
         <v>0</v>
@@ -1623,7 +1585,7 @@
     </row>
     <row r="12" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
-        <v>241</v>
+        <v>160</v>
       </c>
       <c r="B12" s="1">
         <v>0</v>
@@ -1631,7 +1593,7 @@
     </row>
     <row r="13" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
-        <v>240</v>
+        <v>171</v>
       </c>
       <c r="B13" s="1">
         <v>0</v>
@@ -1639,7 +1601,7 @@
     </row>
     <row r="14" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
-        <v>239</v>
+        <v>159</v>
       </c>
       <c r="B14" s="1">
         <v>0</v>
@@ -1647,7 +1609,7 @@
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
-        <v>238</v>
+        <v>172</v>
       </c>
       <c r="B15" s="1">
         <v>0</v>
@@ -1655,7 +1617,7 @@
     </row>
     <row r="16" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
-        <v>237</v>
+        <v>158</v>
       </c>
       <c r="B16" s="1">
         <v>0</v>
@@ -1663,7 +1625,7 @@
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>236</v>
+        <v>173</v>
       </c>
       <c r="B17" s="1">
         <v>0</v>
@@ -1671,7 +1633,7 @@
     </row>
     <row r="18" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
-        <v>235</v>
+        <v>157</v>
       </c>
       <c r="B18" s="1">
         <v>0</v>
@@ -1679,7 +1641,7 @@
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>234</v>
+        <v>156</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
@@ -1695,7 +1657,7 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21" s="5" t="s">
-        <v>233</v>
+        <v>174</v>
       </c>
       <c r="B21" s="1">
         <v>0</v>
@@ -1703,7 +1665,7 @@
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22" s="5" t="s">
-        <v>232</v>
+        <v>155</v>
       </c>
       <c r="B22" s="1">
         <v>1</v>
@@ -1711,7 +1673,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23" s="5" t="s">
-        <v>231</v>
+        <v>175</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -1719,7 +1681,7 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>230</v>
+        <v>154</v>
       </c>
       <c r="B24" s="1">
         <v>1</v>
@@ -1727,7 +1689,7 @@
     </row>
     <row r="25" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
-        <v>229</v>
+        <v>153</v>
       </c>
       <c r="B25" s="1">
         <v>0</v>
@@ -1735,7 +1697,7 @@
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26" s="5" t="s">
-        <v>228</v>
+        <v>152</v>
       </c>
       <c r="B26" s="1">
         <v>1</v>
@@ -1743,7 +1705,7 @@
     </row>
     <row r="27" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
-        <v>227</v>
+        <v>176</v>
       </c>
       <c r="B27" s="1">
         <v>1</v>
@@ -1751,7 +1713,7 @@
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>226</v>
+        <v>151</v>
       </c>
       <c r="B28" s="1">
         <v>1</v>
@@ -1759,7 +1721,7 @@
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>225</v>
+        <v>150</v>
       </c>
       <c r="B29" s="1">
         <v>0</v>
@@ -1767,7 +1729,7 @@
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30" s="5" t="s">
-        <v>224</v>
+        <v>149</v>
       </c>
       <c r="B30" s="1">
         <v>0</v>
@@ -1775,7 +1737,7 @@
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31" s="5" t="s">
-        <v>223</v>
+        <v>148</v>
       </c>
       <c r="B31" s="1">
         <v>0</v>
@@ -1783,7 +1745,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32" s="5" t="s">
-        <v>222</v>
+        <v>147</v>
       </c>
       <c r="B32" s="1">
         <v>0</v>
@@ -1791,7 +1753,7 @@
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33" s="5" t="s">
-        <v>221</v>
+        <v>177</v>
       </c>
       <c r="B33" s="1">
         <v>0</v>
@@ -1799,7 +1761,7 @@
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34" s="5" t="s">
-        <v>220</v>
+        <v>178</v>
       </c>
       <c r="B34" s="1">
         <v>0</v>
@@ -1807,7 +1769,7 @@
     </row>
     <row r="35" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
-        <v>219</v>
+        <v>146</v>
       </c>
       <c r="B35" s="1">
         <v>0</v>
@@ -1815,7 +1777,7 @@
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>218</v>
+        <v>145</v>
       </c>
       <c r="B36" s="1">
         <v>0</v>
@@ -1823,7 +1785,7 @@
     </row>
     <row r="37" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
-        <v>217</v>
+        <v>179</v>
       </c>
       <c r="B37" s="1">
         <v>0</v>
@@ -1831,7 +1793,7 @@
     </row>
     <row r="38" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
-        <v>216</v>
+        <v>180</v>
       </c>
       <c r="B38" s="1">
         <v>0</v>
@@ -1839,7 +1801,7 @@
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A39" s="5" t="s">
-        <v>215</v>
+        <v>144</v>
       </c>
       <c r="B39" s="1">
         <v>0</v>
@@ -1847,7 +1809,7 @@
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>214</v>
+        <v>143</v>
       </c>
       <c r="B40" s="1">
         <v>1</v>
@@ -1855,7 +1817,7 @@
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>213</v>
+        <v>142</v>
       </c>
       <c r="B41" s="1">
         <v>1</v>
@@ -1863,7 +1825,7 @@
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>212</v>
+        <v>181</v>
       </c>
       <c r="B42" s="1">
         <v>1</v>
@@ -1871,7 +1833,7 @@
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A43" s="5" t="s">
-        <v>211</v>
+        <v>182</v>
       </c>
       <c r="B43" s="1">
         <v>0</v>
@@ -1879,7 +1841,7 @@
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>210</v>
+        <v>183</v>
       </c>
       <c r="B44" s="1">
         <v>0</v>
@@ -1887,7 +1849,7 @@
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A45" s="5" t="s">
-        <v>209</v>
+        <v>184</v>
       </c>
       <c r="B45" s="1">
         <v>0</v>
@@ -1895,7 +1857,7 @@
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A46" s="5" t="s">
-        <v>208</v>
+        <v>185</v>
       </c>
       <c r="B46" s="1">
         <v>0</v>
@@ -1903,7 +1865,7 @@
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A47" s="5" t="s">
-        <v>207</v>
+        <v>186</v>
       </c>
       <c r="B47" s="1">
         <v>1</v>
@@ -1911,7 +1873,7 @@
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A48" s="5" t="s">
-        <v>206</v>
+        <v>187</v>
       </c>
       <c r="B48" s="1">
         <v>0</v>
@@ -1919,7 +1881,7 @@
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>205</v>
+        <v>188</v>
       </c>
       <c r="B49" s="1">
         <v>0</v>
@@ -1927,7 +1889,7 @@
     </row>
     <row r="50" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B50" s="1">
         <v>1</v>
@@ -1935,7 +1897,7 @@
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>203</v>
+        <v>190</v>
       </c>
       <c r="B51" s="1">
         <v>0</v>
@@ -1943,7 +1905,7 @@
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="9" t="s">
-        <v>202</v>
+        <v>141</v>
       </c>
       <c r="B52" s="10">
         <v>0</v>
@@ -1951,7 +1913,7 @@
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="9" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="B53" s="10">
         <v>0</v>
@@ -1959,7 +1921,7 @@
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A54" s="9" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B54" s="10">
         <v>0</v>
@@ -1967,7 +1929,7 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A55" s="9" t="s">
-        <v>199</v>
+        <v>140</v>
       </c>
       <c r="B55" s="10">
         <v>0</v>
@@ -1975,7 +1937,7 @@
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A56" s="9" t="s">
-        <v>198</v>
+        <v>139</v>
       </c>
       <c r="B56" s="10">
         <v>1</v>
@@ -1983,7 +1945,7 @@
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A57" s="9" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="B57" s="10">
         <v>1</v>
@@ -1991,7 +1953,7 @@
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A58" s="9" t="s">
-        <v>196</v>
+        <v>138</v>
       </c>
       <c r="B58" s="10">
         <v>1</v>
@@ -1999,7 +1961,7 @@
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A59" s="9" t="s">
-        <v>195</v>
+        <v>137</v>
       </c>
       <c r="B59" s="10">
         <v>1</v>
@@ -2015,7 +1977,7 @@
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A61" s="9" t="s">
-        <v>193</v>
+        <v>195</v>
       </c>
       <c r="B61" s="10">
         <v>1</v>
@@ -2023,7 +1985,7 @@
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A62" s="9" t="s">
-        <v>192</v>
+        <v>196</v>
       </c>
       <c r="B62" s="10">
         <v>1</v>
@@ -2031,7 +1993,7 @@
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A63" s="9" t="s">
-        <v>191</v>
+        <v>136</v>
       </c>
       <c r="B63" s="10">
         <v>1</v>
@@ -2039,7 +2001,7 @@
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A64" s="9" t="s">
-        <v>190</v>
+        <v>135</v>
       </c>
       <c r="B64" s="10">
         <v>1</v>
@@ -2047,7 +2009,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="9" t="s">
-        <v>189</v>
+        <v>134</v>
       </c>
       <c r="B65" s="10">
         <v>1</v>
@@ -2055,7 +2017,7 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A66" s="9" t="s">
-        <v>188</v>
+        <v>133</v>
       </c>
       <c r="B66" s="10">
         <v>1</v>
@@ -2063,7 +2025,7 @@
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A67" s="9" t="s">
-        <v>187</v>
+        <v>132</v>
       </c>
       <c r="B67" s="10">
         <v>1</v>
@@ -2071,7 +2033,7 @@
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A68" s="9" t="s">
-        <v>186</v>
+        <v>197</v>
       </c>
       <c r="B68" s="10">
         <v>0</v>
@@ -2079,7 +2041,7 @@
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A69" s="9" t="s">
-        <v>185</v>
+        <v>131</v>
       </c>
       <c r="B69" s="10">
         <v>1</v>
@@ -2087,7 +2049,7 @@
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A70" s="9" t="s">
-        <v>184</v>
+        <v>198</v>
       </c>
       <c r="B70" s="10">
         <v>1</v>
@@ -2095,7 +2057,7 @@
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A71" s="11" t="s">
-        <v>183</v>
+        <v>130</v>
       </c>
       <c r="B71" s="10">
         <v>1</v>
@@ -2103,7 +2065,7 @@
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A72" s="11" t="s">
-        <v>182</v>
+        <v>129</v>
       </c>
       <c r="B72" s="10">
         <v>1</v>
@@ -2111,7 +2073,7 @@
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A73" s="11" t="s">
-        <v>181</v>
+        <v>128</v>
       </c>
       <c r="B73" s="10">
         <v>1</v>
@@ -2119,7 +2081,7 @@
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A74" s="11" t="s">
-        <v>180</v>
+        <v>127</v>
       </c>
       <c r="B74" s="10">
         <v>1</v>
@@ -2127,7 +2089,7 @@
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A75" s="11" t="s">
-        <v>179</v>
+        <v>126</v>
       </c>
       <c r="B75" s="10">
         <v>0</v>
@@ -2135,7 +2097,7 @@
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A76" s="11" t="s">
-        <v>178</v>
+        <v>125</v>
       </c>
       <c r="B76" s="10">
         <v>0</v>
@@ -2143,7 +2105,7 @@
     </row>
     <row r="77" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
-        <v>177</v>
+        <v>199</v>
       </c>
       <c r="B77" s="10">
         <v>0</v>
@@ -2151,7 +2113,7 @@
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A78" s="11" t="s">
-        <v>176</v>
+        <v>124</v>
       </c>
       <c r="B78" s="10">
         <v>0</v>
@@ -2159,7 +2121,7 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A79" s="11" t="s">
-        <v>175</v>
+        <v>123</v>
       </c>
       <c r="B79" s="10">
         <v>1</v>
@@ -2167,7 +2129,7 @@
     </row>
     <row r="80" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A80" s="8" t="s">
-        <v>174</v>
+        <v>122</v>
       </c>
       <c r="B80" s="10">
         <v>0</v>
@@ -2175,7 +2137,7 @@
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A81" s="11" t="s">
-        <v>173</v>
+        <v>121</v>
       </c>
       <c r="B81" s="10">
         <v>0</v>
@@ -2183,7 +2145,7 @@
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A82" s="11" t="s">
-        <v>172</v>
+        <v>120</v>
       </c>
       <c r="B82" s="10">
         <v>0</v>
@@ -2191,7 +2153,7 @@
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A83" s="11" t="s">
-        <v>171</v>
+        <v>119</v>
       </c>
       <c r="B83" s="10">
         <v>0</v>
@@ -2199,7 +2161,7 @@
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A84" s="11" t="s">
-        <v>170</v>
+        <v>118</v>
       </c>
       <c r="B84" s="10">
         <v>0</v>
@@ -2207,7 +2169,7 @@
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A85" s="11" t="s">
-        <v>169</v>
+        <v>117</v>
       </c>
       <c r="B85" s="10">
         <v>0</v>
@@ -2215,7 +2177,7 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A86" s="11" t="s">
-        <v>168</v>
+        <v>200</v>
       </c>
       <c r="B86" s="10">
         <v>0</v>
@@ -2223,7 +2185,7 @@
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A87" s="11" t="s">
-        <v>167</v>
+        <v>116</v>
       </c>
       <c r="B87" s="10">
         <v>0</v>
@@ -2231,7 +2193,7 @@
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A88" s="11" t="s">
-        <v>166</v>
+        <v>201</v>
       </c>
       <c r="B88" s="10">
         <v>0</v>
@@ -2239,7 +2201,7 @@
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A89" s="11" t="s">
-        <v>165</v>
+        <v>115</v>
       </c>
       <c r="B89" s="10">
         <v>1</v>
@@ -2247,7 +2209,7 @@
     </row>
     <row r="90" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A90" s="12" t="s">
-        <v>164</v>
+        <v>114</v>
       </c>
       <c r="B90" s="10">
         <v>1</v>
@@ -2255,7 +2217,7 @@
     </row>
     <row r="91" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A91" s="12" t="s">
-        <v>163</v>
+        <v>202</v>
       </c>
       <c r="B91" s="10">
         <v>1</v>
@@ -2263,7 +2225,7 @@
     </row>
     <row r="92" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A92" s="12" t="s">
-        <v>162</v>
+        <v>113</v>
       </c>
       <c r="B92" s="10">
         <v>1</v>
@@ -2271,7 +2233,7 @@
     </row>
     <row r="93" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A93" s="12" t="s">
-        <v>161</v>
+        <v>112</v>
       </c>
       <c r="B93" s="10">
         <v>0</v>
@@ -2279,7 +2241,7 @@
     </row>
     <row r="94" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A94" s="12" t="s">
-        <v>160</v>
+        <v>203</v>
       </c>
       <c r="B94" s="10">
         <v>0</v>
@@ -2287,7 +2249,7 @@
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A95" s="11" t="s">
-        <v>159</v>
+        <v>111</v>
       </c>
       <c r="B95" s="10">
         <v>0</v>
@@ -2295,7 +2257,7 @@
     </row>
     <row r="96" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A96" s="12" t="s">
-        <v>158</v>
+        <v>110</v>
       </c>
       <c r="B96" s="10">
         <v>1</v>
@@ -2303,7 +2265,7 @@
     </row>
     <row r="97" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A97" s="12" t="s">
-        <v>157</v>
+        <v>109</v>
       </c>
       <c r="B97" s="10">
         <v>0</v>
@@ -2311,7 +2273,7 @@
     </row>
     <row r="98" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A98" s="12" t="s">
-        <v>156</v>
+        <v>204</v>
       </c>
       <c r="B98" s="10">
         <v>0</v>
@@ -2319,7 +2281,7 @@
     </row>
     <row r="99" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A99" s="12" t="s">
-        <v>155</v>
+        <v>205</v>
       </c>
       <c r="B99" s="10">
         <v>0</v>
@@ -2327,7 +2289,7 @@
     </row>
     <row r="100" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A100" s="12" t="s">
-        <v>154</v>
+        <v>207</v>
       </c>
       <c r="B100" s="10">
         <v>1</v>
@@ -2335,7 +2297,7 @@
     </row>
     <row r="101" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A101" s="12" t="s">
-        <v>153</v>
+        <v>108</v>
       </c>
       <c r="B101" s="10">
         <v>1</v>
@@ -2343,7 +2305,7 @@
     </row>
     <row r="102" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A102" s="12" t="s">
-        <v>152</v>
+        <v>107</v>
       </c>
       <c r="B102" s="10">
         <v>0</v>
@@ -2351,7 +2313,7 @@
     </row>
     <row r="103" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A103" s="12" t="s">
-        <v>151</v>
+        <v>106</v>
       </c>
       <c r="B103" s="10">
         <v>1</v>
@@ -2359,7 +2321,7 @@
     </row>
     <row r="104" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A104" s="8" t="s">
-        <v>150</v>
+        <v>105</v>
       </c>
       <c r="B104" s="10">
         <v>0</v>
@@ -2367,7 +2329,7 @@
     </row>
     <row r="105" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A105" s="8" t="s">
-        <v>149</v>
+        <v>104</v>
       </c>
       <c r="B105" s="10">
         <v>1</v>
@@ -2375,7 +2337,7 @@
     </row>
     <row r="106" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A106" s="8" t="s">
-        <v>148</v>
+        <v>103</v>
       </c>
       <c r="B106" s="10">
         <v>1</v>
@@ -2383,7 +2345,7 @@
     </row>
     <row r="107" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A107" s="8" t="s">
-        <v>147</v>
+        <v>102</v>
       </c>
       <c r="B107" s="10">
         <v>0</v>
@@ -2391,7 +2353,7 @@
     </row>
     <row r="108" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
-        <v>146</v>
+        <v>101</v>
       </c>
       <c r="B108" s="10">
         <v>0</v>
@@ -2399,7 +2361,7 @@
     </row>
     <row r="109" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A109" s="8" t="s">
-        <v>145</v>
+        <v>208</v>
       </c>
       <c r="B109" s="10">
         <v>1</v>
@@ -2407,7 +2369,7 @@
     </row>
     <row r="110" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A110" s="8" t="s">
-        <v>144</v>
+        <v>209</v>
       </c>
       <c r="B110" s="10">
         <v>0</v>
@@ -2415,7 +2377,7 @@
     </row>
     <row r="111" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A111" s="8" t="s">
-        <v>143</v>
+        <v>210</v>
       </c>
       <c r="B111" s="10">
         <v>0</v>
@@ -2423,7 +2385,7 @@
     </row>
     <row r="112" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A112" s="8" t="s">
-        <v>142</v>
+        <v>100</v>
       </c>
       <c r="B112" s="10">
         <v>0</v>
@@ -2431,7 +2393,7 @@
     </row>
     <row r="113" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A113" s="8" t="s">
-        <v>141</v>
+        <v>99</v>
       </c>
       <c r="B113" s="10">
         <v>0</v>
@@ -2439,7 +2401,7 @@
     </row>
     <row r="114" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A114" s="8" t="s">
-        <v>140</v>
+        <v>98</v>
       </c>
       <c r="B114" s="10">
         <v>1</v>
@@ -2447,7 +2409,7 @@
     </row>
     <row r="115" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A115" s="8" t="s">
-        <v>139</v>
+        <v>211</v>
       </c>
       <c r="B115" s="10">
         <v>1</v>
@@ -2455,7 +2417,7 @@
     </row>
     <row r="116" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A116" s="8" t="s">
-        <v>138</v>
+        <v>212</v>
       </c>
       <c r="B116" s="10">
         <v>1</v>
@@ -2463,7 +2425,7 @@
     </row>
     <row r="117" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A117" s="8" t="s">
-        <v>137</v>
+        <v>213</v>
       </c>
       <c r="B117" s="10">
         <v>1</v>
@@ -2471,7 +2433,7 @@
     </row>
     <row r="118" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A118" s="8" t="s">
-        <v>136</v>
+        <v>97</v>
       </c>
       <c r="B118" s="10">
         <v>1</v>
@@ -2479,7 +2441,7 @@
     </row>
     <row r="119" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A119" s="13" t="s">
-        <v>135</v>
+        <v>214</v>
       </c>
       <c r="B119" s="14">
         <v>1</v>
@@ -2487,7 +2449,7 @@
     </row>
     <row r="120" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A120" s="15" t="s">
-        <v>2</v>
+        <v>215</v>
       </c>
       <c r="B120" s="14">
         <v>1</v>
@@ -2495,7 +2457,7 @@
     </row>
     <row r="121" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A121" s="13" t="s">
-        <v>3</v>
+        <v>216</v>
       </c>
       <c r="B121" s="14">
         <v>0</v>
@@ -2503,7 +2465,7 @@
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A122" s="9" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B122" s="14">
         <v>0</v>
@@ -2511,7 +2473,7 @@
     </row>
     <row r="123" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A123" s="13" t="s">
-        <v>5</v>
+        <v>217</v>
       </c>
       <c r="B123" s="14">
         <v>0</v>
@@ -2519,7 +2481,7 @@
     </row>
     <row r="124" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A124" s="13" t="s">
-        <v>6</v>
+        <v>218</v>
       </c>
       <c r="B124" s="14">
         <v>0</v>
@@ -2527,7 +2489,7 @@
     </row>
     <row r="125" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A125" s="13" t="s">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="B125" s="14">
         <v>0</v>
@@ -2535,7 +2497,7 @@
     </row>
     <row r="126" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A126" s="13" t="s">
-        <v>8</v>
+        <v>219</v>
       </c>
       <c r="B126" s="14">
         <v>0</v>
@@ -2543,7 +2505,7 @@
     </row>
     <row r="127" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A127" s="13" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B127" s="14">
         <v>0</v>
@@ -2551,7 +2513,7 @@
     </row>
     <row r="128" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A128" s="13" t="s">
-        <v>10</v>
+        <v>220</v>
       </c>
       <c r="B128" s="14">
         <v>0</v>
@@ -2559,7 +2521,7 @@
     </row>
     <row r="129" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A129" s="13" t="s">
-        <v>11</v>
+        <v>221</v>
       </c>
       <c r="B129" s="14">
         <v>0</v>
@@ -2567,7 +2529,7 @@
     </row>
     <row r="130" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A130" s="13" t="s">
-        <v>12</v>
+        <v>222</v>
       </c>
       <c r="B130" s="14">
         <v>0</v>
@@ -2575,7 +2537,7 @@
     </row>
     <row r="131" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A131" s="13" t="s">
-        <v>13</v>
+        <v>223</v>
       </c>
       <c r="B131" s="14">
         <v>1</v>
@@ -2583,7 +2545,7 @@
     </row>
     <row r="132" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A132" s="13" t="s">
-        <v>14</v>
+        <v>224</v>
       </c>
       <c r="B132" s="14">
         <v>0</v>
@@ -2591,7 +2553,7 @@
     </row>
     <row r="133" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A133" s="13" t="s">
-        <v>15</v>
+        <v>225</v>
       </c>
       <c r="B133" s="14">
         <v>0</v>
@@ -2599,7 +2561,7 @@
     </row>
     <row r="134" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A134" s="13" t="s">
-        <v>16</v>
+        <v>226</v>
       </c>
       <c r="B134" s="14">
         <v>0</v>
@@ -2607,7 +2569,7 @@
     </row>
     <row r="135" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A135" s="13" t="s">
-        <v>17</v>
+        <v>5</v>
       </c>
       <c r="B135" s="14">
         <v>0</v>
@@ -2615,7 +2577,7 @@
     </row>
     <row r="136" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A136" s="13" t="s">
-        <v>18</v>
+        <v>227</v>
       </c>
       <c r="B136" s="14">
         <v>0</v>
@@ -2623,7 +2585,7 @@
     </row>
     <row r="137" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A137" s="13" t="s">
-        <v>19</v>
+        <v>228</v>
       </c>
       <c r="B137" s="14">
         <v>0</v>
@@ -2631,7 +2593,7 @@
     </row>
     <row r="138" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A138" s="13" t="s">
-        <v>20</v>
+        <v>6</v>
       </c>
       <c r="B138" s="14">
         <v>1</v>
@@ -2639,7 +2601,7 @@
     </row>
     <row r="139" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A139" s="13" t="s">
-        <v>21</v>
+        <v>7</v>
       </c>
       <c r="B139" s="14">
         <v>0</v>
@@ -2647,7 +2609,7 @@
     </row>
     <row r="140" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A140" s="13" t="s">
-        <v>22</v>
+        <v>229</v>
       </c>
       <c r="B140" s="14">
         <v>0</v>
@@ -2655,7 +2617,7 @@
     </row>
     <row r="141" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A141" s="13" t="s">
-        <v>23</v>
+        <v>8</v>
       </c>
       <c r="B141" s="14">
         <v>0</v>
@@ -2663,7 +2625,7 @@
     </row>
     <row r="142" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A142" s="13" t="s">
-        <v>24</v>
+        <v>230</v>
       </c>
       <c r="B142" s="14">
         <v>0</v>
@@ -2671,7 +2633,7 @@
     </row>
     <row r="143" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A143" s="13" t="s">
-        <v>25</v>
+        <v>231</v>
       </c>
       <c r="B143" s="14">
         <v>0</v>
@@ -2679,7 +2641,7 @@
     </row>
     <row r="144" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A144" s="13" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="B144" s="14">
         <v>0</v>
@@ -2687,7 +2649,7 @@
     </row>
     <row r="145" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A145" s="13" t="s">
-        <v>27</v>
+        <v>232</v>
       </c>
       <c r="B145" s="14">
         <v>0</v>
@@ -2695,7 +2657,7 @@
     </row>
     <row r="146" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A146" s="13" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="B146" s="14">
         <v>0</v>
@@ -2703,7 +2665,7 @@
     </row>
     <row r="147" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A147" s="13" t="s">
-        <v>29</v>
+        <v>11</v>
       </c>
       <c r="B147" s="14">
         <v>0</v>
@@ -2711,7 +2673,7 @@
     </row>
     <row r="148" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A148" s="13" t="s">
-        <v>30</v>
+        <v>233</v>
       </c>
       <c r="B148" s="14">
         <v>0</v>
@@ -2719,7 +2681,7 @@
     </row>
     <row r="149" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A149" s="13" t="s">
-        <v>31</v>
+        <v>234</v>
       </c>
       <c r="B149" s="14">
         <v>1</v>
@@ -2727,7 +2689,7 @@
     </row>
     <row r="150" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A150" s="13" t="s">
-        <v>32</v>
+        <v>12</v>
       </c>
       <c r="B150" s="14">
         <v>0</v>
@@ -2735,7 +2697,7 @@
     </row>
     <row r="151" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A151" s="13" t="s">
-        <v>33</v>
+        <v>13</v>
       </c>
       <c r="B151" s="14">
         <v>0</v>
@@ -2743,7 +2705,7 @@
     </row>
     <row r="152" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A152" s="13" t="s">
-        <v>34</v>
+        <v>14</v>
       </c>
       <c r="B152" s="10">
         <v>0</v>
@@ -2751,7 +2713,7 @@
     </row>
     <row r="153" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A153" s="13" t="s">
-        <v>35</v>
+        <v>15</v>
       </c>
       <c r="B153" s="10">
         <v>0</v>
@@ -2759,7 +2721,7 @@
     </row>
     <row r="154" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A154" s="13" t="s">
-        <v>36</v>
+        <v>16</v>
       </c>
       <c r="B154" s="10">
         <v>0</v>
@@ -2767,7 +2729,7 @@
     </row>
     <row r="155" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A155" s="13" t="s">
-        <v>37</v>
+        <v>17</v>
       </c>
       <c r="B155" s="10">
         <v>0</v>
@@ -2775,7 +2737,7 @@
     </row>
     <row r="156" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A156" s="13" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="B156" s="10">
         <v>0</v>
@@ -2783,7 +2745,7 @@
     </row>
     <row r="157" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A157" s="13" t="s">
-        <v>39</v>
+        <v>19</v>
       </c>
       <c r="B157" s="10">
         <v>1</v>
@@ -2791,7 +2753,7 @@
     </row>
     <row r="158" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A158" s="13" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="B158" s="10">
         <v>0</v>
@@ -2799,7 +2761,7 @@
     </row>
     <row r="159" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A159" s="13" t="s">
-        <v>41</v>
+        <v>21</v>
       </c>
       <c r="B159" s="10">
         <v>0</v>
@@ -2807,7 +2769,7 @@
     </row>
     <row r="160" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A160" s="13" t="s">
-        <v>42</v>
+        <v>22</v>
       </c>
       <c r="B160" s="10">
         <v>0</v>
@@ -2815,7 +2777,7 @@
     </row>
     <row r="161" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A161" s="13" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="B161" s="10">
         <v>1</v>
@@ -2823,7 +2785,7 @@
     </row>
     <row r="162" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A162" s="13" t="s">
-        <v>44</v>
+        <v>24</v>
       </c>
       <c r="B162" s="10">
         <v>0</v>
@@ -2831,7 +2793,7 @@
     </row>
     <row r="163" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A163" s="13" t="s">
-        <v>45</v>
+        <v>25</v>
       </c>
       <c r="B163" s="10">
         <v>0</v>
@@ -2839,7 +2801,7 @@
     </row>
     <row r="164" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A164" s="16" t="s">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="B164" s="10">
         <v>0</v>
@@ -2847,7 +2809,7 @@
     </row>
     <row r="165" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A165" s="13" t="s">
-        <v>47</v>
+        <v>27</v>
       </c>
       <c r="B165" s="10">
         <v>0</v>
@@ -2855,7 +2817,7 @@
     </row>
     <row r="166" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A166" s="16" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="B166" s="10">
         <v>1</v>
@@ -2863,7 +2825,7 @@
     </row>
     <row r="167" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A167" s="13" t="s">
-        <v>49</v>
+        <v>29</v>
       </c>
       <c r="B167" s="10">
         <v>0</v>
@@ -2871,7 +2833,7 @@
     </row>
     <row r="168" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A168" s="13" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="B168" s="10">
         <v>0</v>
@@ -2879,7 +2841,7 @@
     </row>
     <row r="169" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A169" s="13" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="B169" s="10">
         <v>1</v>
@@ -2887,7 +2849,7 @@
     </row>
     <row r="170" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A170" s="13" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="B170" s="10">
         <v>1</v>
@@ -2895,7 +2857,7 @@
     </row>
     <row r="171" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A171" s="13" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="B171" s="10">
         <v>0</v>
@@ -2903,7 +2865,7 @@
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A172" s="9" t="s">
-        <v>54</v>
+        <v>34</v>
       </c>
       <c r="B172" s="10">
         <v>0</v>
@@ -2911,7 +2873,7 @@
     </row>
     <row r="173" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A173" s="13" t="s">
-        <v>55</v>
+        <v>35</v>
       </c>
       <c r="B173" s="10">
         <v>0</v>
@@ -2919,7 +2881,7 @@
     </row>
     <row r="174" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A174" s="13" t="s">
-        <v>56</v>
+        <v>36</v>
       </c>
       <c r="B174" s="10">
         <v>1</v>
@@ -2927,7 +2889,7 @@
     </row>
     <row r="175" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A175" s="13" t="s">
-        <v>57</v>
+        <v>37</v>
       </c>
       <c r="B175" s="10">
         <v>1</v>
@@ -2935,7 +2897,7 @@
     </row>
     <row r="176" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A176" s="13" t="s">
-        <v>58</v>
+        <v>38</v>
       </c>
       <c r="B176" s="10">
         <v>0</v>
@@ -2943,7 +2905,7 @@
     </row>
     <row r="177" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A177" s="13" t="s">
-        <v>59</v>
+        <v>39</v>
       </c>
       <c r="B177" s="10">
         <v>0</v>
@@ -2951,7 +2913,7 @@
     </row>
     <row r="178" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A178" s="13" t="s">
-        <v>60</v>
+        <v>40</v>
       </c>
       <c r="B178" s="10">
         <v>0</v>
@@ -2959,7 +2921,7 @@
     </row>
     <row r="179" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A179" s="13" t="s">
-        <v>61</v>
+        <v>41</v>
       </c>
       <c r="B179" s="10">
         <v>1</v>
@@ -2967,7 +2929,7 @@
     </row>
     <row r="180" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A180" s="13" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B180" s="10">
         <v>0</v>
@@ -2975,7 +2937,7 @@
     </row>
     <row r="181" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A181" s="13" t="s">
-        <v>63</v>
+        <v>43</v>
       </c>
       <c r="B181" s="10">
         <v>0</v>
@@ -2983,7 +2945,7 @@
     </row>
     <row r="182" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A182" s="13" t="s">
-        <v>64</v>
+        <v>44</v>
       </c>
       <c r="B182" s="10">
         <v>0</v>
@@ -2991,7 +2953,7 @@
     </row>
     <row r="183" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A183" s="13" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="B183" s="10">
         <v>0</v>
@@ -2999,7 +2961,7 @@
     </row>
     <row r="184" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A184" s="13" t="s">
-        <v>66</v>
+        <v>46</v>
       </c>
       <c r="B184" s="10">
         <v>0</v>
@@ -3007,7 +2969,7 @@
     </row>
     <row r="185" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A185" s="13" t="s">
-        <v>67</v>
+        <v>47</v>
       </c>
       <c r="B185" s="10">
         <v>1</v>
@@ -3015,7 +2977,7 @@
     </row>
     <row r="186" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A186" s="13" t="s">
-        <v>68</v>
+        <v>48</v>
       </c>
       <c r="B186" s="10">
         <v>1</v>
@@ -3023,7 +2985,7 @@
     </row>
     <row r="187" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A187" s="13" t="s">
-        <v>69</v>
+        <v>49</v>
       </c>
       <c r="B187" s="10">
         <v>1</v>
@@ -3031,7 +2993,7 @@
     </row>
     <row r="188" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A188" s="13" t="s">
-        <v>70</v>
+        <v>50</v>
       </c>
       <c r="B188" s="10">
         <v>0</v>
@@ -3039,7 +3001,7 @@
     </row>
     <row r="189" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A189" s="13" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="B189" s="10">
         <v>0</v>
@@ -3047,7 +3009,7 @@
     </row>
     <row r="190" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A190" s="16" t="s">
-        <v>72</v>
+        <v>52</v>
       </c>
       <c r="B190" s="10">
         <v>1</v>
@@ -3055,7 +3017,7 @@
     </row>
     <row r="191" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A191" s="13" t="s">
-        <v>73</v>
+        <v>53</v>
       </c>
       <c r="B191" s="10">
         <v>1</v>
@@ -3063,7 +3025,7 @@
     </row>
     <row r="192" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A192" s="13" t="s">
-        <v>74</v>
+        <v>54</v>
       </c>
       <c r="B192" s="10">
         <v>0</v>
@@ -3071,7 +3033,7 @@
     </row>
     <row r="193" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A193" s="13" t="s">
-        <v>75</v>
+        <v>55</v>
       </c>
       <c r="B193" s="10">
         <v>0</v>
@@ -3079,7 +3041,7 @@
     </row>
     <row r="194" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A194" s="13" t="s">
-        <v>76</v>
+        <v>56</v>
       </c>
       <c r="B194" s="10">
         <v>1</v>
@@ -3087,7 +3049,7 @@
     </row>
     <row r="195" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A195" s="13" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
       <c r="B195" s="10">
         <v>1</v>
@@ -3095,7 +3057,7 @@
     </row>
     <row r="196" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A196" s="13" t="s">
-        <v>78</v>
+        <v>58</v>
       </c>
       <c r="B196" s="10">
         <v>1</v>
@@ -3103,7 +3065,7 @@
     </row>
     <row r="197" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A197" s="13" t="s">
-        <v>79</v>
+        <v>59</v>
       </c>
       <c r="B197" s="10">
         <v>1</v>
@@ -3111,7 +3073,7 @@
     </row>
     <row r="198" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A198" s="13" t="s">
-        <v>80</v>
+        <v>60</v>
       </c>
       <c r="B198" s="10">
         <v>0</v>
@@ -3119,7 +3081,7 @@
     </row>
     <row r="199" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A199" s="13" t="s">
-        <v>81</v>
+        <v>61</v>
       </c>
       <c r="B199" s="10">
         <v>0</v>
@@ -3127,7 +3089,7 @@
     </row>
     <row r="200" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A200" s="13" t="s">
-        <v>82</v>
+        <v>62</v>
       </c>
       <c r="B200" s="10">
         <v>0</v>
@@ -3135,7 +3097,7 @@
     </row>
     <row r="201" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A201" s="13" t="s">
-        <v>83</v>
+        <v>63</v>
       </c>
       <c r="B201" s="17">
         <v>0</v>
@@ -3143,7 +3105,7 @@
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A202" s="9" t="s">
-        <v>84</v>
+        <v>64</v>
       </c>
       <c r="B202" s="10">
         <v>0</v>
@@ -3151,7 +3113,7 @@
     </row>
     <row r="203" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A203" s="13" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="B203" s="10">
         <v>0</v>
@@ -3159,7 +3121,7 @@
     </row>
     <row r="204" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A204" s="13" t="s">
-        <v>86</v>
+        <v>66</v>
       </c>
       <c r="B204" s="10">
         <v>0</v>
@@ -3167,7 +3129,7 @@
     </row>
     <row r="205" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A205" s="13" t="s">
-        <v>87</v>
+        <v>67</v>
       </c>
       <c r="B205" s="10">
         <v>0</v>
@@ -3175,7 +3137,7 @@
     </row>
     <row r="206" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A206" s="13" t="s">
-        <v>88</v>
+        <v>68</v>
       </c>
       <c r="B206" s="10">
         <v>0</v>
@@ -3183,7 +3145,7 @@
     </row>
     <row r="207" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A207" s="13" t="s">
-        <v>89</v>
+        <v>69</v>
       </c>
       <c r="B207" s="10">
         <v>0</v>
@@ -3191,7 +3153,7 @@
     </row>
     <row r="208" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A208" s="13" t="s">
-        <v>90</v>
+        <v>70</v>
       </c>
       <c r="B208" s="10">
         <v>0</v>
@@ -3199,7 +3161,7 @@
     </row>
     <row r="209" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A209" s="13" t="s">
-        <v>91</v>
+        <v>71</v>
       </c>
       <c r="B209" s="10">
         <v>0</v>
@@ -3207,7 +3169,7 @@
     </row>
     <row r="210" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A210" s="13" t="s">
-        <v>92</v>
+        <v>72</v>
       </c>
       <c r="B210" s="10">
         <v>0</v>
@@ -3215,7 +3177,7 @@
     </row>
     <row r="211" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A211" s="13" t="s">
-        <v>93</v>
+        <v>73</v>
       </c>
       <c r="B211" s="10">
         <v>0</v>
@@ -3223,7 +3185,7 @@
     </row>
     <row r="212" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A212" s="13" t="s">
-        <v>94</v>
+        <v>74</v>
       </c>
       <c r="B212" s="10">
         <v>0</v>
@@ -3231,7 +3193,7 @@
     </row>
     <row r="213" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A213" s="13" t="s">
-        <v>95</v>
+        <v>75</v>
       </c>
       <c r="B213" s="10">
         <v>0</v>
@@ -3239,7 +3201,7 @@
     </row>
     <row r="214" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A214" s="13" t="s">
-        <v>96</v>
+        <v>76</v>
       </c>
       <c r="B214" s="10">
         <v>1</v>
@@ -3247,7 +3209,7 @@
     </row>
     <row r="215" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A215" s="13" t="s">
-        <v>97</v>
+        <v>77</v>
       </c>
       <c r="B215" s="10">
         <v>0</v>
@@ -3255,7 +3217,7 @@
     </row>
     <row r="216" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A216" s="13" t="s">
-        <v>98</v>
+        <v>78</v>
       </c>
       <c r="B216" s="10">
         <v>1</v>
@@ -3263,7 +3225,7 @@
     </row>
     <row r="217" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A217" s="13" t="s">
-        <v>99</v>
+        <v>79</v>
       </c>
       <c r="B217" s="10">
         <v>1</v>
@@ -3271,7 +3233,7 @@
     </row>
     <row r="218" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A218" s="13" t="s">
-        <v>100</v>
+        <v>80</v>
       </c>
       <c r="B218" s="10">
         <v>1</v>
@@ -3279,7 +3241,7 @@
     </row>
     <row r="219" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A219" s="13" t="s">
-        <v>101</v>
+        <v>81</v>
       </c>
       <c r="B219" s="10">
         <v>0</v>
@@ -3287,7 +3249,7 @@
     </row>
     <row r="220" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A220" s="13" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="B220" s="10">
         <v>0</v>
@@ -3295,7 +3257,7 @@
     </row>
     <row r="221" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A221" s="13" t="s">
-        <v>103</v>
+        <v>83</v>
       </c>
       <c r="B221" s="10">
         <v>0</v>
@@ -3303,7 +3265,7 @@
     </row>
     <row r="222" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A222" s="13" t="s">
-        <v>104</v>
+        <v>84</v>
       </c>
       <c r="B222" s="10">
         <v>0</v>
@@ -3311,7 +3273,7 @@
     </row>
     <row r="223" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A223" s="13" t="s">
-        <v>105</v>
+        <v>251</v>
       </c>
       <c r="B223" s="10">
         <v>1</v>
@@ -3319,7 +3281,7 @@
     </row>
     <row r="224" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A224" s="13" t="s">
-        <v>106</v>
+        <v>85</v>
       </c>
       <c r="B224" s="10">
         <v>1</v>
@@ -3327,7 +3289,7 @@
     </row>
     <row r="225" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A225" s="13" t="s">
-        <v>107</v>
+        <v>86</v>
       </c>
       <c r="B225" s="10">
         <v>0</v>
@@ -3335,7 +3297,7 @@
     </row>
     <row r="226" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A226" s="13" t="s">
-        <v>108</v>
+        <v>250</v>
       </c>
       <c r="B226" s="10">
         <v>0</v>
@@ -3343,7 +3305,7 @@
     </row>
     <row r="227" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A227" s="13" t="s">
-        <v>109</v>
+        <v>249</v>
       </c>
       <c r="B227" s="10">
         <v>1</v>
@@ -3351,7 +3313,7 @@
     </row>
     <row r="228" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A228" s="13" t="s">
-        <v>110</v>
+        <v>248</v>
       </c>
       <c r="B228" s="10">
         <v>0</v>
@@ -3359,7 +3321,7 @@
     </row>
     <row r="229" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A229" s="13" t="s">
-        <v>111</v>
+        <v>87</v>
       </c>
       <c r="B229" s="10">
         <v>0</v>
@@ -3367,7 +3329,7 @@
     </row>
     <row r="230" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A230" s="13" t="s">
-        <v>112</v>
+        <v>247</v>
       </c>
       <c r="B230" s="10">
         <v>1</v>
@@ -3375,7 +3337,7 @@
     </row>
     <row r="231" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A231" s="13" t="s">
-        <v>113</v>
+        <v>88</v>
       </c>
       <c r="B231" s="10">
         <v>1</v>
@@ -3383,7 +3345,7 @@
     </row>
     <row r="232" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A232" s="13" t="s">
-        <v>114</v>
+        <v>246</v>
       </c>
       <c r="B232" s="10">
         <v>1</v>
@@ -3391,7 +3353,7 @@
     </row>
     <row r="233" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A233" s="13" t="s">
-        <v>115</v>
+        <v>245</v>
       </c>
       <c r="B233" s="10">
         <v>0</v>
@@ -3399,7 +3361,7 @@
     </row>
     <row r="234" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A234" s="13" t="s">
-        <v>116</v>
+        <v>244</v>
       </c>
       <c r="B234" s="10">
         <v>0</v>
@@ -3407,7 +3369,7 @@
     </row>
     <row r="235" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A235" s="13" t="s">
-        <v>117</v>
+        <v>243</v>
       </c>
       <c r="B235" s="10">
         <v>0</v>
@@ -3415,7 +3377,7 @@
     </row>
     <row r="236" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A236" s="13" t="s">
-        <v>118</v>
+        <v>242</v>
       </c>
       <c r="B236" s="10">
         <v>1</v>
@@ -3423,7 +3385,7 @@
     </row>
     <row r="237" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A237" s="13" t="s">
-        <v>119</v>
+        <v>241</v>
       </c>
       <c r="B237" s="10">
         <v>1</v>
@@ -3431,7 +3393,7 @@
     </row>
     <row r="238" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A238" s="13" t="s">
-        <v>120</v>
+        <v>89</v>
       </c>
       <c r="B238" s="10">
         <v>0</v>
@@ -3439,7 +3401,7 @@
     </row>
     <row r="239" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A239" s="13" t="s">
-        <v>121</v>
+        <v>90</v>
       </c>
       <c r="B239" s="10">
         <v>1</v>
@@ -3447,7 +3409,7 @@
     </row>
     <row r="240" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A240" s="13" t="s">
-        <v>122</v>
+        <v>91</v>
       </c>
       <c r="B240" s="10">
         <v>0</v>
@@ -3455,7 +3417,7 @@
     </row>
     <row r="241" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A241" s="13" t="s">
-        <v>123</v>
+        <v>240</v>
       </c>
       <c r="B241" s="10">
         <v>0</v>
@@ -3463,7 +3425,7 @@
     </row>
     <row r="242" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A242" s="13" t="s">
-        <v>124</v>
+        <v>239</v>
       </c>
       <c r="B242" s="10">
         <v>1</v>
@@ -3471,7 +3433,7 @@
     </row>
     <row r="243" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A243" s="13" t="s">
-        <v>125</v>
+        <v>238</v>
       </c>
       <c r="B243" s="10">
         <v>1</v>
@@ -3479,7 +3441,7 @@
     </row>
     <row r="244" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A244" s="13" t="s">
-        <v>126</v>
+        <v>237</v>
       </c>
       <c r="B244" s="10">
         <v>0</v>
@@ -3487,7 +3449,7 @@
     </row>
     <row r="245" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A245" s="13" t="s">
-        <v>127</v>
+        <v>92</v>
       </c>
       <c r="B245" s="10">
         <v>1</v>
@@ -3495,7 +3457,7 @@
     </row>
     <row r="246" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A246" s="13" t="s">
-        <v>128</v>
+        <v>236</v>
       </c>
       <c r="B246" s="10">
         <v>0</v>
@@ -3503,7 +3465,7 @@
     </row>
     <row r="247" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A247" s="13" t="s">
-        <v>129</v>
+        <v>235</v>
       </c>
       <c r="B247" s="10">
         <v>1</v>
@@ -3511,7 +3473,7 @@
     </row>
     <row r="248" spans="1:2" ht="17.25" x14ac:dyDescent="0.3">
       <c r="A248" s="13" t="s">
-        <v>130</v>
+        <v>93</v>
       </c>
       <c r="B248" s="10">
         <v>1</v>
@@ -3519,7 +3481,7 @@
     </row>
     <row r="249" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A249" s="13" t="s">
-        <v>131</v>
+        <v>94</v>
       </c>
       <c r="B249" s="10">
         <v>0</v>
@@ -3527,7 +3489,7 @@
     </row>
     <row r="250" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A250" s="13" t="s">
-        <v>132</v>
+        <v>95</v>
       </c>
       <c r="B250" s="10">
         <v>1</v>
@@ -3535,7 +3497,7 @@
     </row>
     <row r="251" spans="1:2" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A251" s="13" t="s">
-        <v>133</v>
+        <v>169</v>
       </c>
       <c r="B251" s="10">
         <v>0</v>

</xml_diff>